<commit_message>
Implementazione del contorno della mappa
In MapVisualizer.cs:
- Aggiunto il metodo GenerateMapBorder per la creazione del bordo della mappa
- Aggiunto il metodo GenerateOuterMap per la creazione del contorno della mappa
- Riorganizzate le directory per la gestione degli asset
</commit_message>
<xml_diff>
--- a/Genetic Map Generation/Data/GAData.xlsx
+++ b/Genetic Map Generation/Data/GAData.xlsx
@@ -429,7 +429,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="0">
-        <v>67</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8">
@@ -437,7 +437,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="0">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9">
@@ -445,7 +445,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="0">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10">
@@ -453,7 +453,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="0">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11">
@@ -461,7 +461,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="0">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12">
@@ -469,7 +469,7 @@
         <v>6</v>
       </c>
       <c r="D12" s="0">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13">
@@ -477,7 +477,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="0">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -486,7 +486,7 @@
         <v>8</v>
       </c>
       <c r="D14" s="0">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15">
@@ -494,7 +494,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="0">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16">
@@ -502,7 +502,7 @@
         <v>10</v>
       </c>
       <c r="D16" s="0">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17">
@@ -510,7 +510,7 @@
         <v>11</v>
       </c>
       <c r="D17" s="0">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18">
@@ -518,7 +518,7 @@
         <v>12</v>
       </c>
       <c r="D18" s="0">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19">
@@ -526,7 +526,7 @@
         <v>13</v>
       </c>
       <c r="D19" s="0">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20">
@@ -534,7 +534,7 @@
         <v>14</v>
       </c>
       <c r="D20" s="0">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21">
@@ -542,7 +542,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="0">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22">
@@ -550,7 +550,7 @@
         <v>16</v>
       </c>
       <c r="D22" s="0">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23">
@@ -558,7 +558,7 @@
         <v>17</v>
       </c>
       <c r="D23" s="0">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24">
@@ -566,7 +566,7 @@
         <v>18</v>
       </c>
       <c r="D24" s="0">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25">
@@ -574,7 +574,7 @@
         <v>19</v>
       </c>
       <c r="D25" s="0">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26">
@@ -582,7 +582,7 @@
         <v>20</v>
       </c>
       <c r="D26" s="0">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27">
@@ -590,7 +590,7 @@
         <v>21</v>
       </c>
       <c r="D27" s="0">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28">
@@ -598,7 +598,7 @@
         <v>22</v>
       </c>
       <c r="D28" s="0">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29">
@@ -606,7 +606,7 @@
         <v>23</v>
       </c>
       <c r="D29" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30">
@@ -614,7 +614,7 @@
         <v>24</v>
       </c>
       <c r="D30" s="0">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31">
@@ -622,7 +622,7 @@
         <v>25</v>
       </c>
       <c r="D31" s="0">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32">
@@ -638,7 +638,7 @@
         <v>27</v>
       </c>
       <c r="D33" s="0">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34">
@@ -646,7 +646,7 @@
         <v>28</v>
       </c>
       <c r="D34" s="0">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35">
@@ -654,7 +654,7 @@
         <v>29</v>
       </c>
       <c r="D35" s="0">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36">
@@ -662,7 +662,7 @@
         <v>30</v>
       </c>
       <c r="D36" s="0">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37">
@@ -670,7 +670,7 @@
         <v>31</v>
       </c>
       <c r="D37" s="0">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38">
@@ -678,7 +678,7 @@
         <v>32</v>
       </c>
       <c r="D38" s="0">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39">
@@ -686,7 +686,7 @@
         <v>33</v>
       </c>
       <c r="D39" s="0">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40">
@@ -694,7 +694,7 @@
         <v>34</v>
       </c>
       <c r="D40" s="0">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41">
@@ -702,7 +702,7 @@
         <v>35</v>
       </c>
       <c r="D41" s="0">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42">
@@ -710,7 +710,7 @@
         <v>36</v>
       </c>
       <c r="D42" s="0">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43">
@@ -718,7 +718,7 @@
         <v>37</v>
       </c>
       <c r="D43" s="0">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44">
@@ -726,7 +726,7 @@
         <v>38</v>
       </c>
       <c r="D44" s="0">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45">
@@ -734,7 +734,7 @@
         <v>39</v>
       </c>
       <c r="D45" s="0">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46">
@@ -742,7 +742,7 @@
         <v>40</v>
       </c>
       <c r="D46" s="0">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47">
@@ -750,7 +750,7 @@
         <v>41</v>
       </c>
       <c r="D47" s="0">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48">
@@ -758,7 +758,7 @@
         <v>42</v>
       </c>
       <c r="D48" s="0">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49">
@@ -766,7 +766,7 @@
         <v>43</v>
       </c>
       <c r="D49" s="0">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="50">
@@ -774,7 +774,7 @@
         <v>44</v>
       </c>
       <c r="D50" s="0">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51">
@@ -782,7 +782,7 @@
         <v>45</v>
       </c>
       <c r="D51" s="0">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52">
@@ -790,7 +790,7 @@
         <v>46</v>
       </c>
       <c r="D52" s="0">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53">
@@ -798,7 +798,7 @@
         <v>47</v>
       </c>
       <c r="D53" s="0">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54">
@@ -806,7 +806,7 @@
         <v>48</v>
       </c>
       <c r="D54" s="0">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="55">
@@ -814,7 +814,7 @@
         <v>49</v>
       </c>
       <c r="D55" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56">
@@ -822,7 +822,7 @@
         <v>50</v>
       </c>
       <c r="D56" s="0">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementazione angolazioni camera e visualizzazione dati in UI
- Aggiunta la funzionalità per cambiare la modalità di visualizzazione della mappa (3D o 2D)
- Aggiunta la funzionalità per mostrare nell'UI i dati inerenti alla mappa e all'algoritmo genetico
</commit_message>
<xml_diff>
--- a/Genetic Map Generation/Data/GAData.xlsx
+++ b/Genetic Map Generation/Data/GAData.xlsx
@@ -15,8 +15,10 @@
   <sheets>
     <sheet name="Foglio1" sheetId="16" r:id="rId1"/>
     <sheet name="Foglio2" sheetId="17" r:id="rId2"/>
+    <sheet name="Foglio3" sheetId="18" r:id="rId6"/>
+    <sheet name="Foglio4" sheetId="19" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Configurazione Algoritmo Genetico</t>
   </si>
@@ -88,7 +90,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,7 +129,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -258,31 +261,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="2" applyFont="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="7" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="13" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -631,7 +688,7 @@
     <col min="8" max="8" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5">
       <c r="B5" s="12" t="s">
         <v>0</v>
       </c>
@@ -643,7 +700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6">
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
@@ -657,7 +714,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7">
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
@@ -671,7 +728,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8">
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
@@ -685,7 +742,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9">
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
@@ -699,7 +756,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10">
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
@@ -713,7 +770,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="11">
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
@@ -727,7 +784,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="12">
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
@@ -741,7 +798,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13">
       <c r="B13" s="2" t="s">
         <v>10</v>
       </c>
@@ -755,7 +812,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14">
       <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
@@ -769,7 +826,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15">
       <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
@@ -783,7 +840,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16">
       <c r="B16" s="2" t="s">
         <v>13</v>
       </c>
@@ -797,7 +854,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17">
       <c r="B17" s="3" t="s">
         <v>14</v>
       </c>
@@ -811,7 +868,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18">
       <c r="G18" s="1">
         <v>13</v>
       </c>
@@ -819,7 +876,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19">
       <c r="G19" s="1">
         <v>14</v>
       </c>
@@ -827,7 +884,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20">
       <c r="G20" s="1">
         <v>15</v>
       </c>
@@ -835,7 +892,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21">
       <c r="G21" s="1">
         <v>16</v>
       </c>
@@ -843,7 +900,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22">
       <c r="G22" s="1">
         <v>17</v>
       </c>
@@ -851,7 +908,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23">
       <c r="G23" s="1">
         <v>18</v>
       </c>
@@ -859,7 +916,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24">
       <c r="G24" s="1">
         <v>19</v>
       </c>
@@ -867,7 +924,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="25">
       <c r="G25" s="1">
         <v>20</v>
       </c>
@@ -875,15 +932,1185 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="26">
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells>
     <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName=""/>
+  <dimension ref="B5:O17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="9.4" customWidth="1"/>
+    <col min="7" max="7" width="10.6" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
+    <col min="11" max="11" width="21" customWidth="1"/>
+    <col min="12" max="12" width="21" customWidth="1"/>
+    <col min="13" max="13" width="21" customWidth="1"/>
+    <col min="14" max="14" width="21" customWidth="1"/>
+    <col min="15" max="15" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5">
+      <c r="B5" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="G5" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="O5" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="20">
+        <v>10</v>
+      </c>
+      <c r="G6" s="22">
+        <v>1</v>
+      </c>
+      <c r="H6" s="22">
+        <v>87</v>
+      </c>
+      <c r="I6" s="23">
+        <v>88</v>
+      </c>
+      <c r="J6" s="23">
+        <v>86</v>
+      </c>
+      <c r="K6" s="23">
+        <v>85</v>
+      </c>
+      <c r="L6" s="23">
+        <v>92</v>
+      </c>
+      <c r="M6" s="23">
+        <v>92</v>
+      </c>
+      <c r="N6" s="23">
+        <v>91</v>
+      </c>
+      <c r="O6" s="23">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="20">
+        <v>10</v>
+      </c>
+      <c r="G7" s="22">
+        <v>2</v>
+      </c>
+      <c r="H7" s="22">
+        <v>78</v>
+      </c>
+      <c r="I7" s="23">
+        <v>75</v>
+      </c>
+      <c r="J7" s="23">
+        <v>77</v>
+      </c>
+      <c r="K7" s="23">
+        <v>69</v>
+      </c>
+      <c r="L7" s="23">
+        <v>90</v>
+      </c>
+      <c r="M7" s="23">
+        <v>84</v>
+      </c>
+      <c r="N7" s="23">
+        <v>89</v>
+      </c>
+      <c r="O7" s="23">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="20">
+        <v>100</v>
+      </c>
+      <c r="G8" s="22">
+        <v>3</v>
+      </c>
+      <c r="H8" s="22">
+        <v>86</v>
+      </c>
+      <c r="I8" s="23">
+        <v>76</v>
+      </c>
+      <c r="J8" s="23">
+        <v>75</v>
+      </c>
+      <c r="K8" s="23">
+        <v>82</v>
+      </c>
+      <c r="L8" s="23">
+        <v>72</v>
+      </c>
+      <c r="M8" s="23">
+        <v>75</v>
+      </c>
+      <c r="N8" s="23">
+        <v>75</v>
+      </c>
+      <c r="O8" s="23">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="20">
+        <v>15</v>
+      </c>
+      <c r="G9" s="22">
+        <v>4</v>
+      </c>
+      <c r="H9" s="22">
+        <v>86</v>
+      </c>
+      <c r="I9" s="23">
+        <v>64</v>
+      </c>
+      <c r="J9" s="23">
+        <v>80</v>
+      </c>
+      <c r="K9" s="23">
+        <v>77</v>
+      </c>
+      <c r="L9" s="23">
+        <v>74</v>
+      </c>
+      <c r="M9" s="23">
+        <v>75</v>
+      </c>
+      <c r="N9" s="23">
+        <v>78</v>
+      </c>
+      <c r="O9" s="23">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="20">
+        <v>6</v>
+      </c>
+      <c r="G10" s="22">
+        <v>5</v>
+      </c>
+      <c r="H10" s="22">
+        <v>82</v>
+      </c>
+      <c r="I10" s="23">
+        <v>76</v>
+      </c>
+      <c r="J10" s="23">
+        <v>79</v>
+      </c>
+      <c r="K10" s="23">
+        <v>79</v>
+      </c>
+      <c r="L10" s="23">
+        <v>79</v>
+      </c>
+      <c r="M10" s="23">
+        <v>80</v>
+      </c>
+      <c r="N10" s="23">
+        <v>77</v>
+      </c>
+      <c r="O10" s="23">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="20">
+        <v>12</v>
+      </c>
+      <c r="G11" s="22">
+        <v>6</v>
+      </c>
+      <c r="H11" s="22">
+        <v>83</v>
+      </c>
+      <c r="I11" s="23">
+        <v>78</v>
+      </c>
+      <c r="J11" s="23">
+        <v>76</v>
+      </c>
+      <c r="K11" s="23">
+        <v>74</v>
+      </c>
+      <c r="L11" s="23">
+        <v>76</v>
+      </c>
+      <c r="M11" s="23">
+        <v>71</v>
+      </c>
+      <c r="N11" s="23">
+        <v>71</v>
+      </c>
+      <c r="O11" s="23">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="20">
+        <v>1</v>
+      </c>
+      <c r="G12" s="22">
+        <v>7</v>
+      </c>
+      <c r="H12" s="22">
+        <v>78</v>
+      </c>
+      <c r="I12" s="23">
+        <v>68</v>
+      </c>
+      <c r="J12" s="23">
+        <v>69</v>
+      </c>
+      <c r="K12" s="23">
+        <v>72</v>
+      </c>
+      <c r="L12" s="23">
+        <v>70</v>
+      </c>
+      <c r="M12" s="23">
+        <v>75</v>
+      </c>
+      <c r="N12" s="23">
+        <v>71</v>
+      </c>
+      <c r="O12" s="23">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="20">
+        <v>1</v>
+      </c>
+      <c r="G13" s="22">
+        <v>8</v>
+      </c>
+      <c r="H13" s="22">
+        <v>81</v>
+      </c>
+      <c r="I13" s="23">
+        <v>73</v>
+      </c>
+      <c r="J13" s="23">
+        <v>74</v>
+      </c>
+      <c r="K13" s="23">
+        <v>77</v>
+      </c>
+      <c r="L13" s="23">
+        <v>77</v>
+      </c>
+      <c r="M13" s="23">
+        <v>74</v>
+      </c>
+      <c r="N13" s="23">
+        <v>78</v>
+      </c>
+      <c r="O13" s="23">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="20">
+        <v>1</v>
+      </c>
+      <c r="G14" s="22">
+        <v>9</v>
+      </c>
+      <c r="H14" s="22">
+        <v>75</v>
+      </c>
+      <c r="I14" s="23">
+        <v>75</v>
+      </c>
+      <c r="J14" s="23">
+        <v>80</v>
+      </c>
+      <c r="K14" s="23">
+        <v>78</v>
+      </c>
+      <c r="L14" s="23">
+        <v>74</v>
+      </c>
+      <c r="M14" s="23">
+        <v>76</v>
+      </c>
+      <c r="N14" s="23">
+        <v>76</v>
+      </c>
+      <c r="O14" s="23">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="20">
+        <v>10</v>
+      </c>
+      <c r="G15" s="22">
+        <v>10</v>
+      </c>
+      <c r="H15" s="22">
+        <v>81</v>
+      </c>
+      <c r="I15" s="23">
+        <v>84</v>
+      </c>
+      <c r="J15" s="23">
+        <v>73</v>
+      </c>
+      <c r="K15" s="23">
+        <v>77</v>
+      </c>
+      <c r="L15" s="23">
+        <v>72</v>
+      </c>
+      <c r="M15" s="23">
+        <v>75</v>
+      </c>
+      <c r="N15" s="23">
+        <v>74</v>
+      </c>
+      <c r="O15" s="23">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="20">
+        <v>10</v>
+      </c>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="21">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells>
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName=""/>
+  <dimension ref="B5:L36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="9.4" customWidth="1"/>
+    <col min="7" max="7" width="10.6" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
+    <col min="11" max="11" width="21" customWidth="1"/>
+    <col min="12" max="12" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5">
+      <c r="B5" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="G5" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="20">
+        <v>10</v>
+      </c>
+      <c r="G6" s="22">
+        <v>1</v>
+      </c>
+      <c r="H6" s="22">
+        <v>133</v>
+      </c>
+      <c r="I6" s="23">
+        <v>121</v>
+      </c>
+      <c r="J6" s="23">
+        <v>125</v>
+      </c>
+      <c r="K6" s="23">
+        <v>124</v>
+      </c>
+      <c r="L6" s="23">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="20">
+        <v>30</v>
+      </c>
+      <c r="G7" s="22">
+        <v>2</v>
+      </c>
+      <c r="H7" s="22">
+        <v>128</v>
+      </c>
+      <c r="I7" s="23">
+        <v>132</v>
+      </c>
+      <c r="J7" s="23">
+        <v>135</v>
+      </c>
+      <c r="K7" s="23">
+        <v>134</v>
+      </c>
+      <c r="L7" s="23">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="20">
+        <v>100</v>
+      </c>
+      <c r="G8" s="22">
+        <v>3</v>
+      </c>
+      <c r="H8" s="22">
+        <v>136</v>
+      </c>
+      <c r="I8" s="23">
+        <v>142</v>
+      </c>
+      <c r="J8" s="23">
+        <v>133</v>
+      </c>
+      <c r="K8" s="23">
+        <v>135</v>
+      </c>
+      <c r="L8" s="23">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="20">
+        <v>15</v>
+      </c>
+      <c r="G9" s="22">
+        <v>4</v>
+      </c>
+      <c r="H9" s="22">
+        <v>138</v>
+      </c>
+      <c r="I9" s="23">
+        <v>125</v>
+      </c>
+      <c r="J9" s="23">
+        <v>137</v>
+      </c>
+      <c r="K9" s="23">
+        <v>139</v>
+      </c>
+      <c r="L9" s="23">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="20">
+        <v>6</v>
+      </c>
+      <c r="G10" s="22">
+        <v>5</v>
+      </c>
+      <c r="H10" s="22">
+        <v>137</v>
+      </c>
+      <c r="I10" s="23">
+        <v>133</v>
+      </c>
+      <c r="J10" s="23">
+        <v>141</v>
+      </c>
+      <c r="K10" s="23">
+        <v>131</v>
+      </c>
+      <c r="L10" s="23">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="20">
+        <v>12</v>
+      </c>
+      <c r="G11" s="22">
+        <v>6</v>
+      </c>
+      <c r="H11" s="22">
+        <v>141</v>
+      </c>
+      <c r="I11" s="23">
+        <v>137</v>
+      </c>
+      <c r="J11" s="23">
+        <v>137</v>
+      </c>
+      <c r="K11" s="23">
+        <v>137</v>
+      </c>
+      <c r="L11" s="23">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="20">
+        <v>1</v>
+      </c>
+      <c r="G12" s="22">
+        <v>7</v>
+      </c>
+      <c r="H12" s="22">
+        <v>141</v>
+      </c>
+      <c r="I12" s="23">
+        <v>143</v>
+      </c>
+      <c r="J12" s="23">
+        <v>153</v>
+      </c>
+      <c r="K12" s="23">
+        <v>142</v>
+      </c>
+      <c r="L12" s="23">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="20">
+        <v>1</v>
+      </c>
+      <c r="G13" s="22">
+        <v>8</v>
+      </c>
+      <c r="H13" s="22">
+        <v>144</v>
+      </c>
+      <c r="I13" s="23">
+        <v>137</v>
+      </c>
+      <c r="J13" s="23">
+        <v>137</v>
+      </c>
+      <c r="K13" s="23">
+        <v>143</v>
+      </c>
+      <c r="L13" s="23">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="20">
+        <v>1</v>
+      </c>
+      <c r="G14" s="22">
+        <v>9</v>
+      </c>
+      <c r="H14" s="22">
+        <v>150</v>
+      </c>
+      <c r="I14" s="23">
+        <v>135</v>
+      </c>
+      <c r="J14" s="23">
+        <v>146</v>
+      </c>
+      <c r="K14" s="23">
+        <v>143</v>
+      </c>
+      <c r="L14" s="23">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="20">
+        <v>15</v>
+      </c>
+      <c r="G15" s="22">
+        <v>10</v>
+      </c>
+      <c r="H15" s="22">
+        <v>148</v>
+      </c>
+      <c r="I15" s="23">
+        <v>136</v>
+      </c>
+      <c r="J15" s="23">
+        <v>147</v>
+      </c>
+      <c r="K15" s="23">
+        <v>147</v>
+      </c>
+      <c r="L15" s="23">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="20">
+        <v>15</v>
+      </c>
+      <c r="G16" s="22">
+        <v>11</v>
+      </c>
+      <c r="H16" s="22">
+        <v>147</v>
+      </c>
+      <c r="I16" s="23">
+        <v>138</v>
+      </c>
+      <c r="J16" s="23">
+        <v>147</v>
+      </c>
+      <c r="K16" s="23">
+        <v>142</v>
+      </c>
+      <c r="L16" s="23">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="21">
+        <v>15</v>
+      </c>
+      <c r="G17" s="22">
+        <v>12</v>
+      </c>
+      <c r="H17" s="22">
+        <v>150</v>
+      </c>
+      <c r="I17" s="23">
+        <v>136</v>
+      </c>
+      <c r="J17" s="23">
+        <v>149</v>
+      </c>
+      <c r="K17" s="23">
+        <v>149</v>
+      </c>
+      <c r="L17" s="23">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="G18" s="22">
+        <v>13</v>
+      </c>
+      <c r="H18" s="22">
+        <v>149</v>
+      </c>
+      <c r="I18" s="23">
+        <v>132</v>
+      </c>
+      <c r="J18" s="23">
+        <v>148</v>
+      </c>
+      <c r="K18" s="23">
+        <v>141</v>
+      </c>
+      <c r="L18" s="23">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="G19" s="22">
+        <v>14</v>
+      </c>
+      <c r="H19" s="22">
+        <v>143</v>
+      </c>
+      <c r="I19" s="23">
+        <v>143</v>
+      </c>
+      <c r="J19" s="23">
+        <v>142</v>
+      </c>
+      <c r="K19" s="23">
+        <v>156</v>
+      </c>
+      <c r="L19" s="23">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="G20" s="22">
+        <v>15</v>
+      </c>
+      <c r="H20" s="22">
+        <v>150</v>
+      </c>
+      <c r="I20" s="23">
+        <v>157</v>
+      </c>
+      <c r="J20" s="23">
+        <v>147</v>
+      </c>
+      <c r="K20" s="23">
+        <v>154</v>
+      </c>
+      <c r="L20" s="23">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="G21" s="22">
+        <v>16</v>
+      </c>
+      <c r="H21" s="22">
+        <v>149</v>
+      </c>
+      <c r="I21" s="23">
+        <v>132</v>
+      </c>
+      <c r="J21" s="23">
+        <v>146</v>
+      </c>
+      <c r="K21" s="23">
+        <v>141</v>
+      </c>
+      <c r="L21" s="23">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="G22" s="22">
+        <v>17</v>
+      </c>
+      <c r="H22" s="22">
+        <v>141</v>
+      </c>
+      <c r="I22" s="23">
+        <v>139</v>
+      </c>
+      <c r="J22" s="23">
+        <v>147</v>
+      </c>
+      <c r="K22" s="23">
+        <v>149</v>
+      </c>
+      <c r="L22" s="23">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="G23" s="22">
+        <v>18</v>
+      </c>
+      <c r="H23" s="22">
+        <v>143</v>
+      </c>
+      <c r="I23" s="23">
+        <v>145</v>
+      </c>
+      <c r="J23" s="23">
+        <v>146</v>
+      </c>
+      <c r="K23" s="23">
+        <v>150</v>
+      </c>
+      <c r="L23" s="23">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="G24" s="22">
+        <v>19</v>
+      </c>
+      <c r="H24" s="22">
+        <v>145</v>
+      </c>
+      <c r="I24" s="23">
+        <v>143</v>
+      </c>
+      <c r="J24" s="23">
+        <v>147</v>
+      </c>
+      <c r="K24" s="23">
+        <v>142</v>
+      </c>
+      <c r="L24" s="23">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="G25" s="22">
+        <v>20</v>
+      </c>
+      <c r="H25" s="22">
+        <v>152</v>
+      </c>
+      <c r="I25" s="23">
+        <v>141</v>
+      </c>
+      <c r="J25" s="23">
+        <v>139</v>
+      </c>
+      <c r="K25" s="23">
+        <v>144</v>
+      </c>
+      <c r="L25" s="23">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="G26" s="22">
+        <v>21</v>
+      </c>
+      <c r="H26" s="22">
+        <v>144</v>
+      </c>
+      <c r="I26" s="23">
+        <v>145</v>
+      </c>
+      <c r="J26" s="23">
+        <v>143</v>
+      </c>
+      <c r="K26" s="23">
+        <v>138</v>
+      </c>
+      <c r="L26" s="23">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="G27" s="22">
+        <v>22</v>
+      </c>
+      <c r="H27" s="22">
+        <v>141</v>
+      </c>
+      <c r="I27" s="23">
+        <v>136</v>
+      </c>
+      <c r="J27" s="23">
+        <v>145</v>
+      </c>
+      <c r="K27" s="23">
+        <v>148</v>
+      </c>
+      <c r="L27" s="23">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="G28" s="22">
+        <v>23</v>
+      </c>
+      <c r="H28" s="22">
+        <v>143</v>
+      </c>
+      <c r="I28" s="23">
+        <v>138</v>
+      </c>
+      <c r="J28" s="23">
+        <v>146</v>
+      </c>
+      <c r="K28" s="23">
+        <v>145</v>
+      </c>
+      <c r="L28" s="23">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="G29" s="22">
+        <v>24</v>
+      </c>
+      <c r="H29" s="22">
+        <v>142</v>
+      </c>
+      <c r="I29" s="23">
+        <v>142</v>
+      </c>
+      <c r="J29" s="23">
+        <v>146</v>
+      </c>
+      <c r="K29" s="23">
+        <v>147</v>
+      </c>
+      <c r="L29" s="23">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="G30" s="22">
+        <v>25</v>
+      </c>
+      <c r="H30" s="22">
+        <v>142</v>
+      </c>
+      <c r="I30" s="23">
+        <v>138</v>
+      </c>
+      <c r="J30" s="23">
+        <v>148</v>
+      </c>
+      <c r="K30" s="23">
+        <v>150</v>
+      </c>
+      <c r="L30" s="23">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="G31" s="22">
+        <v>26</v>
+      </c>
+      <c r="H31" s="22">
+        <v>144</v>
+      </c>
+      <c r="I31" s="23">
+        <v>137</v>
+      </c>
+      <c r="J31" s="23">
+        <v>143</v>
+      </c>
+      <c r="K31" s="23">
+        <v>146</v>
+      </c>
+      <c r="L31" s="23">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="G32" s="22">
+        <v>27</v>
+      </c>
+      <c r="H32" s="22">
+        <v>151</v>
+      </c>
+      <c r="I32" s="23">
+        <v>143</v>
+      </c>
+      <c r="J32" s="23">
+        <v>148</v>
+      </c>
+      <c r="K32" s="23">
+        <v>151</v>
+      </c>
+      <c r="L32" s="23">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="G33" s="22">
+        <v>28</v>
+      </c>
+      <c r="H33" s="22">
+        <v>143</v>
+      </c>
+      <c r="I33" s="23">
+        <v>140</v>
+      </c>
+      <c r="J33" s="23">
+        <v>149</v>
+      </c>
+      <c r="K33" s="23">
+        <v>145</v>
+      </c>
+      <c r="L33" s="23">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="G34" s="22">
+        <v>29</v>
+      </c>
+      <c r="H34" s="22">
+        <v>146</v>
+      </c>
+      <c r="I34" s="23">
+        <v>140</v>
+      </c>
+      <c r="J34" s="23">
+        <v>146</v>
+      </c>
+      <c r="K34" s="23">
+        <v>145</v>
+      </c>
+      <c r="L34" s="23">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="G35" s="22">
+        <v>30</v>
+      </c>
+      <c r="H35" s="22">
+        <v>141</v>
+      </c>
+      <c r="I35" s="23">
+        <v>139</v>
+      </c>
+      <c r="J35" s="23">
+        <v>135</v>
+      </c>
+      <c r="K35" s="23">
+        <v>149</v>
+      </c>
+      <c r="L35" s="23">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="23"/>
+      <c r="L36" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells>
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
+  <headerFooter/>
 </worksheet>
 </file>
 
@@ -904,7 +2131,7 @@
     <col min="9" max="12" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="5">
       <c r="B5" s="14" t="s">
         <v>0</v>
       </c>
@@ -928,7 +2155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="6">
       <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
@@ -954,7 +2181,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="7">
       <c r="B7" s="6" t="s">
         <v>4</v>
       </c>
@@ -980,7 +2207,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="8">
       <c r="B8" s="6" t="s">
         <v>5</v>
       </c>
@@ -1006,7 +2233,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="9">
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
@@ -1033,7 +2260,7 @@
       </c>
       <c r="AC9" s="10"/>
     </row>
-    <row r="10" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="10">
       <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
@@ -1059,7 +2286,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="11">
       <c r="B11" s="6" t="s">
         <v>8</v>
       </c>
@@ -1085,7 +2312,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="12">
       <c r="B12" s="6" t="s">
         <v>9</v>
       </c>
@@ -1111,7 +2338,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="13">
       <c r="B13" s="6" t="s">
         <v>10</v>
       </c>
@@ -1137,7 +2364,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="14">
       <c r="B14" s="6" t="s">
         <v>11</v>
       </c>
@@ -1163,7 +2390,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="15">
       <c r="B15" s="6" t="s">
         <v>12</v>
       </c>
@@ -1189,7 +2416,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="16">
       <c r="B16" s="6" t="s">
         <v>13</v>
       </c>
@@ -1215,7 +2442,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="17">
       <c r="B17" s="7" t="s">
         <v>14</v>
       </c>
@@ -1241,7 +2468,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="18">
       <c r="G18" s="1">
         <v>13</v>
       </c>
@@ -1261,7 +2488,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="19">
       <c r="G19" s="1">
         <v>14</v>
       </c>
@@ -1281,7 +2508,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="20">
       <c r="G20" s="1">
         <v>15</v>
       </c>
@@ -1301,7 +2528,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="21">
       <c r="G21" s="1">
         <v>16</v>
       </c>
@@ -1321,7 +2548,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="22">
       <c r="G22" s="1">
         <v>17</v>
       </c>
@@ -1341,7 +2568,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="23">
       <c r="G23" s="1">
         <v>18</v>
       </c>
@@ -1361,7 +2588,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="24">
       <c r="G24" s="1">
         <v>19</v>
       </c>
@@ -1381,7 +2608,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="25">
       <c r="G25" s="1">
         <v>20</v>
       </c>
@@ -1401,7 +2628,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="26">
       <c r="G26" s="1">
         <v>21</v>
       </c>
@@ -1421,7 +2648,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="27">
       <c r="G27" s="1">
         <v>22</v>
       </c>
@@ -1441,7 +2668,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="28">
       <c r="G28" s="1">
         <v>23</v>
       </c>
@@ -1461,7 +2688,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="29">
       <c r="G29" s="1">
         <v>24</v>
       </c>
@@ -1481,7 +2708,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="30">
       <c r="G30" s="1">
         <v>25</v>
       </c>
@@ -1501,7 +2728,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="31">
       <c r="G31" s="1">
         <v>26</v>
       </c>
@@ -1521,7 +2748,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="32">
       <c r="G32" s="1">
         <v>27</v>
       </c>
@@ -1541,7 +2768,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="33">
       <c r="G33" s="1">
         <v>28</v>
       </c>
@@ -1561,7 +2788,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="34">
       <c r="G34" s="1">
         <v>29</v>
       </c>
@@ -1581,7 +2808,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="35">
       <c r="G35" s="1">
         <v>30</v>
       </c>
@@ -1601,7 +2828,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="36">
       <c r="G36" s="1">
         <v>31</v>
       </c>
@@ -1621,7 +2848,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="37">
       <c r="G37" s="1">
         <v>32</v>
       </c>
@@ -1641,7 +2868,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="38">
       <c r="G38" s="1">
         <v>33</v>
       </c>
@@ -1661,7 +2888,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="39">
       <c r="G39" s="1">
         <v>34</v>
       </c>
@@ -1681,7 +2908,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="40">
       <c r="G40" s="1">
         <v>35</v>
       </c>
@@ -1701,7 +2928,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="41">
       <c r="G41" s="1">
         <v>36</v>
       </c>
@@ -1721,7 +2948,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="42">
       <c r="G42" s="1">
         <v>37</v>
       </c>
@@ -1741,7 +2968,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="43">
       <c r="G43" s="1">
         <v>38</v>
       </c>
@@ -1761,7 +2988,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="44">
       <c r="G44" s="1">
         <v>39</v>
       </c>
@@ -1781,7 +3008,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="45">
       <c r="G45" s="1">
         <v>40</v>
       </c>
@@ -1801,7 +3028,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="46">
       <c r="G46" s="1">
         <v>41</v>
       </c>
@@ -1821,7 +3048,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="47">
       <c r="G47" s="1">
         <v>42</v>
       </c>
@@ -1841,7 +3068,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="48">
       <c r="G48" s="1">
         <v>43</v>
       </c>
@@ -1861,7 +3088,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="49">
       <c r="G49" s="1">
         <v>44</v>
       </c>
@@ -1881,7 +3108,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="50">
       <c r="G50" s="1">
         <v>45</v>
       </c>
@@ -1901,7 +3128,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="51">
       <c r="G51" s="1">
         <v>46</v>
       </c>
@@ -1921,7 +3148,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="52">
       <c r="G52" s="1">
         <v>47</v>
       </c>
@@ -1941,7 +3168,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="53" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="53">
       <c r="G53" s="1">
         <v>48</v>
       </c>
@@ -1961,7 +3188,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="54">
       <c r="G54" s="1">
         <v>49</v>
       </c>
@@ -1981,7 +3208,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="55" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="55">
       <c r="G55" s="1">
         <v>50</v>
       </c>
@@ -2001,7 +3228,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="56">
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
@@ -2010,9 +3237,10 @@
       <c r="L56" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells>
     <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implementata la costruzione della strada con delay
- Aggiunto il metodo GenerateRoadOnDelay in MapVisualizer per generare la strada con un delay
- Modificati i parametri del metodo GenerateMap per ottenere il path per la costruzione della strada
</commit_message>
<xml_diff>
--- a/Genetic Map Generation/Data/GAData.xlsx
+++ b/Genetic Map Generation/Data/GAData.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Configurazione Algoritmo Genetico</t>
   </si>
@@ -119,6 +119,18 @@
   </si>
   <si>
     <t>00:00:00:64302</t>
+  </si>
+  <si>
+    <t>00:00:00:53272</t>
+  </si>
+  <si>
+    <t>00:00:00:48693</t>
+  </si>
+  <si>
+    <t>00:00:00:51418</t>
+  </si>
+  <si>
+    <t>00:00:00:54981</t>
   </si>
 </sst>
 </file>
@@ -4523,7 +4535,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="B5:K41"/>
+  <dimension ref="B5:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I5" sqref="I5:I35"/>
@@ -4538,6 +4550,10 @@
     <col min="9" max="9" width="21" customWidth="1"/>
     <col min="10" max="10" width="21" customWidth="1"/>
     <col min="11" max="11" width="21" customWidth="1"/>
+    <col min="12" max="12" width="21" customWidth="1"/>
+    <col min="13" max="13" width="21" customWidth="1"/>
+    <col min="14" max="14" width="21" customWidth="1"/>
+    <col min="15" max="15" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5">
@@ -4560,6 +4576,18 @@
       <c r="K5" s="39" t="s">
         <v>2</v>
       </c>
+      <c r="L5" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="O5" s="39" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="0" t="s">
@@ -4583,6 +4611,18 @@
       <c r="K6" s="40">
         <v>91</v>
       </c>
+      <c r="L6" s="40">
+        <v>90</v>
+      </c>
+      <c r="M6" s="40">
+        <v>93</v>
+      </c>
+      <c r="N6" s="40">
+        <v>88</v>
+      </c>
+      <c r="O6" s="40">
+        <v>91</v>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="0" t="s">
@@ -4606,6 +4646,18 @@
       <c r="K7" s="40">
         <v>80</v>
       </c>
+      <c r="L7" s="40">
+        <v>78</v>
+      </c>
+      <c r="M7" s="40">
+        <v>85</v>
+      </c>
+      <c r="N7" s="40">
+        <v>81</v>
+      </c>
+      <c r="O7" s="40">
+        <v>80</v>
+      </c>
     </row>
     <row r="8">
       <c r="B8" s="0" t="s">
@@ -4629,6 +4681,18 @@
       <c r="K8" s="40">
         <v>70</v>
       </c>
+      <c r="L8" s="40">
+        <v>75</v>
+      </c>
+      <c r="M8" s="40">
+        <v>78</v>
+      </c>
+      <c r="N8" s="40">
+        <v>84</v>
+      </c>
+      <c r="O8" s="40">
+        <v>78</v>
+      </c>
     </row>
     <row r="9">
       <c r="B9" s="0" t="s">
@@ -4652,6 +4716,18 @@
       <c r="K9" s="40">
         <v>78</v>
       </c>
+      <c r="L9" s="40">
+        <v>72</v>
+      </c>
+      <c r="M9" s="40">
+        <v>81</v>
+      </c>
+      <c r="N9" s="40">
+        <v>77</v>
+      </c>
+      <c r="O9" s="40">
+        <v>77</v>
+      </c>
     </row>
     <row r="10">
       <c r="B10" s="0" t="s">
@@ -4675,6 +4751,18 @@
       <c r="K10" s="40">
         <v>73</v>
       </c>
+      <c r="L10" s="40">
+        <v>72</v>
+      </c>
+      <c r="M10" s="40">
+        <v>84</v>
+      </c>
+      <c r="N10" s="40">
+        <v>74</v>
+      </c>
+      <c r="O10" s="40">
+        <v>76</v>
+      </c>
     </row>
     <row r="11">
       <c r="B11" s="0" t="s">
@@ -4698,6 +4786,18 @@
       <c r="K11" s="40">
         <v>75</v>
       </c>
+      <c r="L11" s="40">
+        <v>75</v>
+      </c>
+      <c r="M11" s="40">
+        <v>78</v>
+      </c>
+      <c r="N11" s="40">
+        <v>76</v>
+      </c>
+      <c r="O11" s="40">
+        <v>73</v>
+      </c>
     </row>
     <row r="12">
       <c r="B12" s="0" t="s">
@@ -4721,6 +4821,18 @@
       <c r="K12" s="40">
         <v>79</v>
       </c>
+      <c r="L12" s="40">
+        <v>76</v>
+      </c>
+      <c r="M12" s="40">
+        <v>76</v>
+      </c>
+      <c r="N12" s="40">
+        <v>74</v>
+      </c>
+      <c r="O12" s="40">
+        <v>71</v>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="0" t="s">
@@ -4744,6 +4856,18 @@
       <c r="K13" s="40">
         <v>76</v>
       </c>
+      <c r="L13" s="40">
+        <v>79</v>
+      </c>
+      <c r="M13" s="40">
+        <v>80</v>
+      </c>
+      <c r="N13" s="40">
+        <v>84</v>
+      </c>
+      <c r="O13" s="40">
+        <v>78</v>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="0" t="s">
@@ -4767,6 +4891,18 @@
       <c r="K14" s="40">
         <v>79</v>
       </c>
+      <c r="L14" s="40">
+        <v>76</v>
+      </c>
+      <c r="M14" s="40">
+        <v>81</v>
+      </c>
+      <c r="N14" s="40">
+        <v>79</v>
+      </c>
+      <c r="O14" s="40">
+        <v>77</v>
+      </c>
     </row>
     <row r="15">
       <c r="B15" s="0" t="s">
@@ -4790,6 +4926,18 @@
       <c r="K15" s="40">
         <v>80</v>
       </c>
+      <c r="L15" s="40">
+        <v>81</v>
+      </c>
+      <c r="M15" s="40">
+        <v>78</v>
+      </c>
+      <c r="N15" s="40">
+        <v>74</v>
+      </c>
+      <c r="O15" s="40">
+        <v>73</v>
+      </c>
     </row>
     <row r="16">
       <c r="B16" s="0" t="s">
@@ -4813,6 +4961,18 @@
       <c r="K16" s="40">
         <v>82</v>
       </c>
+      <c r="L16" s="40">
+        <v>77</v>
+      </c>
+      <c r="M16" s="40">
+        <v>76</v>
+      </c>
+      <c r="N16" s="40">
+        <v>76</v>
+      </c>
+      <c r="O16" s="40">
+        <v>79</v>
+      </c>
     </row>
     <row r="17">
       <c r="B17" s="0" t="s">
@@ -4836,6 +4996,18 @@
       <c r="K17" s="40">
         <v>75</v>
       </c>
+      <c r="L17" s="40">
+        <v>72</v>
+      </c>
+      <c r="M17" s="40">
+        <v>83</v>
+      </c>
+      <c r="N17" s="40">
+        <v>81</v>
+      </c>
+      <c r="O17" s="40">
+        <v>71</v>
+      </c>
     </row>
     <row r="18">
       <c r="G18" s="1">
@@ -4853,6 +5025,18 @@
       <c r="K18" s="40">
         <v>76</v>
       </c>
+      <c r="L18" s="40">
+        <v>80</v>
+      </c>
+      <c r="M18" s="40">
+        <v>71</v>
+      </c>
+      <c r="N18" s="40">
+        <v>72</v>
+      </c>
+      <c r="O18" s="40">
+        <v>78</v>
+      </c>
     </row>
     <row r="19">
       <c r="G19" s="1">
@@ -4870,6 +5054,18 @@
       <c r="K19" s="40">
         <v>78</v>
       </c>
+      <c r="L19" s="40">
+        <v>74</v>
+      </c>
+      <c r="M19" s="40">
+        <v>83</v>
+      </c>
+      <c r="N19" s="40">
+        <v>80</v>
+      </c>
+      <c r="O19" s="40">
+        <v>76</v>
+      </c>
     </row>
     <row r="20">
       <c r="G20" s="1">
@@ -4887,6 +5083,18 @@
       <c r="K20" s="40">
         <v>75</v>
       </c>
+      <c r="L20" s="40">
+        <v>75</v>
+      </c>
+      <c r="M20" s="40">
+        <v>72</v>
+      </c>
+      <c r="N20" s="40">
+        <v>70</v>
+      </c>
+      <c r="O20" s="40">
+        <v>75</v>
+      </c>
     </row>
     <row r="21">
       <c r="G21" s="1">
@@ -4904,6 +5112,18 @@
       <c r="K21" s="40">
         <v>77</v>
       </c>
+      <c r="L21" s="40">
+        <v>73</v>
+      </c>
+      <c r="M21" s="40">
+        <v>74</v>
+      </c>
+      <c r="N21" s="40">
+        <v>81</v>
+      </c>
+      <c r="O21" s="40">
+        <v>72</v>
+      </c>
     </row>
     <row r="22">
       <c r="G22" s="1">
@@ -4921,6 +5141,18 @@
       <c r="K22" s="40">
         <v>75</v>
       </c>
+      <c r="L22" s="40">
+        <v>79</v>
+      </c>
+      <c r="M22" s="40">
+        <v>80</v>
+      </c>
+      <c r="N22" s="40">
+        <v>75</v>
+      </c>
+      <c r="O22" s="40">
+        <v>83</v>
+      </c>
     </row>
     <row r="23">
       <c r="G23" s="1">
@@ -4938,6 +5170,18 @@
       <c r="K23" s="40">
         <v>70</v>
       </c>
+      <c r="L23" s="40">
+        <v>74</v>
+      </c>
+      <c r="M23" s="40">
+        <v>86</v>
+      </c>
+      <c r="N23" s="40">
+        <v>78</v>
+      </c>
+      <c r="O23" s="40">
+        <v>78</v>
+      </c>
     </row>
     <row r="24">
       <c r="G24" s="1">
@@ -4955,6 +5199,18 @@
       <c r="K24" s="40">
         <v>77</v>
       </c>
+      <c r="L24" s="40">
+        <v>77</v>
+      </c>
+      <c r="M24" s="40">
+        <v>78</v>
+      </c>
+      <c r="N24" s="40">
+        <v>77</v>
+      </c>
+      <c r="O24" s="40">
+        <v>77</v>
+      </c>
     </row>
     <row r="25">
       <c r="G25" s="1">
@@ -4972,6 +5228,18 @@
       <c r="K25" s="40">
         <v>74</v>
       </c>
+      <c r="L25" s="40">
+        <v>74</v>
+      </c>
+      <c r="M25" s="40">
+        <v>76</v>
+      </c>
+      <c r="N25" s="40">
+        <v>86</v>
+      </c>
+      <c r="O25" s="40">
+        <v>76</v>
+      </c>
     </row>
     <row r="26">
       <c r="G26" s="1">
@@ -4989,6 +5257,18 @@
       <c r="K26" s="40">
         <v>74</v>
       </c>
+      <c r="L26" s="40">
+        <v>69</v>
+      </c>
+      <c r="M26" s="40">
+        <v>74</v>
+      </c>
+      <c r="N26" s="40">
+        <v>72</v>
+      </c>
+      <c r="O26" s="40">
+        <v>76</v>
+      </c>
     </row>
     <row r="27">
       <c r="G27" s="1">
@@ -5006,6 +5286,18 @@
       <c r="K27" s="40">
         <v>73</v>
       </c>
+      <c r="L27" s="40">
+        <v>74</v>
+      </c>
+      <c r="M27" s="40">
+        <v>77</v>
+      </c>
+      <c r="N27" s="40">
+        <v>77</v>
+      </c>
+      <c r="O27" s="40">
+        <v>78</v>
+      </c>
     </row>
     <row r="28">
       <c r="G28" s="1">
@@ -5023,6 +5315,18 @@
       <c r="K28" s="40">
         <v>77</v>
       </c>
+      <c r="L28" s="40">
+        <v>77</v>
+      </c>
+      <c r="M28" s="40">
+        <v>83</v>
+      </c>
+      <c r="N28" s="40">
+        <v>80</v>
+      </c>
+      <c r="O28" s="40">
+        <v>80</v>
+      </c>
     </row>
     <row r="29">
       <c r="G29" s="1">
@@ -5040,6 +5344,18 @@
       <c r="K29" s="40">
         <v>73</v>
       </c>
+      <c r="L29" s="40">
+        <v>78</v>
+      </c>
+      <c r="M29" s="40">
+        <v>78</v>
+      </c>
+      <c r="N29" s="40">
+        <v>73</v>
+      </c>
+      <c r="O29" s="40">
+        <v>73</v>
+      </c>
     </row>
     <row r="30">
       <c r="G30" s="1">
@@ -5057,6 +5373,18 @@
       <c r="K30" s="40">
         <v>77</v>
       </c>
+      <c r="L30" s="40">
+        <v>82</v>
+      </c>
+      <c r="M30" s="40">
+        <v>81</v>
+      </c>
+      <c r="N30" s="40">
+        <v>73</v>
+      </c>
+      <c r="O30" s="40">
+        <v>73</v>
+      </c>
     </row>
     <row r="31">
       <c r="G31" s="27" t="s">
@@ -5074,6 +5402,18 @@
       <c r="K31" s="41">
         <v>91</v>
       </c>
+      <c r="L31" s="41">
+        <v>90</v>
+      </c>
+      <c r="M31" s="41">
+        <v>93</v>
+      </c>
+      <c r="N31" s="41">
+        <v>88</v>
+      </c>
+      <c r="O31" s="41">
+        <v>91</v>
+      </c>
     </row>
     <row r="32">
       <c r="G32" s="27" t="s">
@@ -5091,6 +5431,18 @@
       <c r="K32" s="41">
         <v>17</v>
       </c>
+      <c r="L32" s="41">
+        <v>23</v>
+      </c>
+      <c r="M32" s="41">
+        <v>24</v>
+      </c>
+      <c r="N32" s="41">
+        <v>24</v>
+      </c>
+      <c r="O32" s="41">
+        <v>16</v>
+      </c>
     </row>
     <row r="33">
       <c r="G33" s="27" t="s">
@@ -5108,6 +5460,18 @@
       <c r="K33" s="41">
         <v>11</v>
       </c>
+      <c r="L33" s="41">
+        <v>10</v>
+      </c>
+      <c r="M33" s="41">
+        <v>12</v>
+      </c>
+      <c r="N33" s="41">
+        <v>11</v>
+      </c>
+      <c r="O33" s="41">
+        <v>10</v>
+      </c>
     </row>
     <row r="34">
       <c r="G34" s="27" t="s">
@@ -5125,6 +5489,18 @@
       <c r="K34" s="41">
         <v>63</v>
       </c>
+      <c r="L34" s="41">
+        <v>57</v>
+      </c>
+      <c r="M34" s="41">
+        <v>57</v>
+      </c>
+      <c r="N34" s="41">
+        <v>53</v>
+      </c>
+      <c r="O34" s="41">
+        <v>65</v>
+      </c>
     </row>
     <row r="35">
       <c r="G35" s="27" t="s">
@@ -5141,6 +5517,18 @@
       </c>
       <c r="K35" s="41" t="s">
         <v>25</v>
+      </c>
+      <c r="L35" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="M35" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="N35" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="O35" s="41" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="36">

</xml_diff>

<commit_message>
Miglioramenti UI e reset mappa
- Miglioramenti generali all'UI
- Aggiunta la finestra per selezionare i parametri dell'algoritmo genetico
- Aggiunto il metodo ClearMapVisual per rigenerare la mappa con parametri diversi
</commit_message>
<xml_diff>
--- a/Genetic Map Generation/Data/GAData.xlsx
+++ b/Genetic Map Generation/Data/GAData.xlsx
@@ -15,6 +15,13 @@
   <sheets>
     <sheet name="Foglio1" sheetId="16" r:id="rId1"/>
     <sheet name="Foglio2" sheetId="17" r:id="rId2"/>
+    <sheet name="Foglio3" sheetId="18" r:id="rId6"/>
+    <sheet name="Foglio4" sheetId="19" r:id="rId7"/>
+    <sheet name="Foglio5" sheetId="20" r:id="rId8"/>
+    <sheet name="Foglio6" sheetId="21" r:id="rId9"/>
+    <sheet name="Foglio7" sheetId="22" r:id="rId10"/>
+    <sheet name="Foglio8" sheetId="23" r:id="rId11"/>
+    <sheet name="Foglio9" sheetId="24" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
   <extLst>
@@ -37,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Configurazione Algoritmo Genetico</t>
   </si>
@@ -113,6 +120,54 @@
   <si>
     <t>00:00:00:11903</t>
   </si>
+  <si>
+    <t>00:00:00:11559</t>
+  </si>
+  <si>
+    <t>00:00:00:00000</t>
+  </si>
+  <si>
+    <t>00:00:00:13965</t>
+  </si>
+  <si>
+    <t>00:00:00:12336</t>
+  </si>
+  <si>
+    <t>00:00:00:08280</t>
+  </si>
+  <si>
+    <t>00:00:00:10475</t>
+  </si>
+  <si>
+    <t>selectionMethod</t>
+  </si>
+  <si>
+    <t>RouletteWheel</t>
+  </si>
+  <si>
+    <t>crossoverMethod</t>
+  </si>
+  <si>
+    <t>SinglePoint</t>
+  </si>
+  <si>
+    <t>mutationMethod</t>
+  </si>
+  <si>
+    <t>BitFlip</t>
+  </si>
+  <si>
+    <t>00:00:00:19218</t>
+  </si>
+  <si>
+    <t>00:00:00:08308</t>
+  </si>
+  <si>
+    <t>00:00:00:09320</t>
+  </si>
+  <si>
+    <t>00:00:00:11640</t>
+  </si>
 </sst>
 </file>
 
@@ -149,7 +204,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -261,11 +316,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -292,6 +389,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="10" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="11" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -898,6 +1005,792 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName=""/>
+  <dimension ref="B5:H40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="9.4" customWidth="1"/>
+    <col min="7" max="7" width="20.3" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5">
+      <c r="B5" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="G5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="0">
+        <v>20</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13">
+        <v>9.701492309570312</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="0">
+        <v>30</v>
+      </c>
+      <c r="G7" s="13">
+        <v>2</v>
+      </c>
+      <c r="H7" s="13">
+        <v>12.283581733703613</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="0">
+        <v>100</v>
+      </c>
+      <c r="G8" s="13">
+        <v>3</v>
+      </c>
+      <c r="H8" s="13">
+        <v>14.850746154785156</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="0">
+        <v>5</v>
+      </c>
+      <c r="G9" s="13">
+        <v>4</v>
+      </c>
+      <c r="H9" s="13">
+        <v>20.597015380859375</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="0">
+        <v>6</v>
+      </c>
+      <c r="G10" s="13">
+        <v>5</v>
+      </c>
+      <c r="H10" s="13">
+        <v>19.17910385131836</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="0">
+        <v>12</v>
+      </c>
+      <c r="G11" s="13">
+        <v>6</v>
+      </c>
+      <c r="H11" s="13">
+        <v>17.46268653869629</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="0">
+        <v>19</v>
+      </c>
+      <c r="G12" s="13">
+        <v>7</v>
+      </c>
+      <c r="H12" s="13">
+        <v>18.26865577697754</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="0">
+        <v>19</v>
+      </c>
+      <c r="G13" s="13">
+        <v>8</v>
+      </c>
+      <c r="H13" s="13">
+        <v>22.865671157836914</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="0">
+        <v>29</v>
+      </c>
+      <c r="G14" s="13">
+        <v>9</v>
+      </c>
+      <c r="H14" s="13">
+        <v>22.865671157836914</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="0">
+        <v>10</v>
+      </c>
+      <c r="G15" s="13">
+        <v>10</v>
+      </c>
+      <c r="H15" s="13">
+        <v>24.298507690429688</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="0">
+        <v>10</v>
+      </c>
+      <c r="G16" s="13">
+        <v>11</v>
+      </c>
+      <c r="H16" s="13">
+        <v>24.850746154785156</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="0">
+        <v>2</v>
+      </c>
+      <c r="G17" s="13">
+        <v>12</v>
+      </c>
+      <c r="H17" s="13">
+        <v>24.567163467407227</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="0">
+        <v>5</v>
+      </c>
+      <c r="G18" s="13">
+        <v>13</v>
+      </c>
+      <c r="H18" s="13">
+        <v>24.582090377807617</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="G19" s="13">
+        <v>14</v>
+      </c>
+      <c r="H19" s="13">
+        <v>22.298507690429688</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="G20" s="13">
+        <v>15</v>
+      </c>
+      <c r="H20" s="13">
+        <v>24.014925003051758</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="G21" s="13">
+        <v>16</v>
+      </c>
+      <c r="H21" s="13">
+        <v>23.701492309570312</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="G22" s="13">
+        <v>17</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="G23" s="13">
+        <v>18</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="G24" s="13">
+        <v>19</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="G25" s="13">
+        <v>20</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="G26" s="13">
+        <v>21</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="G27" s="13">
+        <v>22</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="G28" s="13">
+        <v>23</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="G29" s="13">
+        <v>24</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="G30" s="13">
+        <v>25</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="G31" s="13">
+        <v>26</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="G32" s="13">
+        <v>27</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="G33" s="13">
+        <v>28</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="G34" s="13">
+        <v>29</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="G35" s="13">
+        <v>30</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="G36" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" s="14">
+        <v>24.850746154785156</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="G37" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" s="14">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="G38" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="G39" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" s="14">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="G40" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells>
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName=""/>
+  <dimension ref="B5:H40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="9.4" customWidth="1"/>
+    <col min="7" max="7" width="20.3" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5">
+      <c r="B5" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="G5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="0">
+        <v>20</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="0">
+        <v>30</v>
+      </c>
+      <c r="G7" s="13">
+        <v>2</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="0">
+        <v>100</v>
+      </c>
+      <c r="G8" s="13">
+        <v>3</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="0">
+        <v>5</v>
+      </c>
+      <c r="G9" s="13">
+        <v>4</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="0">
+        <v>6</v>
+      </c>
+      <c r="G10" s="13">
+        <v>5</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="0">
+        <v>12</v>
+      </c>
+      <c r="G11" s="13">
+        <v>6</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="0">
+        <v>0</v>
+      </c>
+      <c r="G12" s="13">
+        <v>7</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="0">
+        <v>0</v>
+      </c>
+      <c r="G13" s="13">
+        <v>8</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="0">
+        <v>0</v>
+      </c>
+      <c r="G14" s="13">
+        <v>9</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="0">
+        <v>10</v>
+      </c>
+      <c r="G15" s="13">
+        <v>10</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="0">
+        <v>10</v>
+      </c>
+      <c r="G16" s="13">
+        <v>11</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="0">
+        <v>2</v>
+      </c>
+      <c r="G17" s="13">
+        <v>12</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="0">
+        <v>5</v>
+      </c>
+      <c r="G18" s="13">
+        <v>13</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="G19" s="13">
+        <v>14</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="G20" s="13">
+        <v>15</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="G21" s="13">
+        <v>16</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="G22" s="13">
+        <v>17</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="G23" s="13">
+        <v>18</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="G24" s="13">
+        <v>19</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="G25" s="13">
+        <v>20</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="G26" s="13">
+        <v>21</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="G27" s="13">
+        <v>22</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="G28" s="13">
+        <v>23</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="G29" s="13">
+        <v>24</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="G30" s="13">
+        <v>25</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="G31" s="13">
+        <v>26</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="G32" s="13">
+        <v>27</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="G33" s="13">
+        <v>28</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="G34" s="13">
+        <v>29</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="G35" s="13">
+        <v>30</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="G36" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="G37" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="G38" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="G39" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="G40" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells>
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B5:J40"/>
@@ -1507,4 +2400,2968 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName=""/>
+  <dimension ref="B5:H40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="9.4" customWidth="1"/>
+    <col min="7" max="7" width="20.3" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5">
+      <c r="B5" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="G5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="0">
+        <v>20</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13">
+        <v>14.784615516662598</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="0">
+        <v>30</v>
+      </c>
+      <c r="G7" s="13">
+        <v>2</v>
+      </c>
+      <c r="H7" s="13">
+        <v>13.7384614944458</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="0">
+        <v>100</v>
+      </c>
+      <c r="G8" s="13">
+        <v>3</v>
+      </c>
+      <c r="H8" s="13">
+        <v>17.184616088867188</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="0">
+        <v>5</v>
+      </c>
+      <c r="G9" s="13">
+        <v>4</v>
+      </c>
+      <c r="H9" s="13">
+        <v>17.676923751831055</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="0">
+        <v>6</v>
+      </c>
+      <c r="G10" s="13">
+        <v>5</v>
+      </c>
+      <c r="H10" s="13">
+        <v>19.21538543701172</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="0">
+        <v>12</v>
+      </c>
+      <c r="G11" s="13">
+        <v>6</v>
+      </c>
+      <c r="H11" s="13">
+        <v>25.461538314819336</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="0">
+        <v>14</v>
+      </c>
+      <c r="G12" s="13">
+        <v>7</v>
+      </c>
+      <c r="H12" s="13">
+        <v>20.230770111083984</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="0">
+        <v>22</v>
+      </c>
+      <c r="G13" s="13">
+        <v>8</v>
+      </c>
+      <c r="H13" s="13">
+        <v>22.015384674072266</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="0">
+        <v>29</v>
+      </c>
+      <c r="G14" s="13">
+        <v>9</v>
+      </c>
+      <c r="H14" s="13">
+        <v>22.72307777404785</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="0">
+        <v>10</v>
+      </c>
+      <c r="G15" s="13">
+        <v>10</v>
+      </c>
+      <c r="H15" s="13">
+        <v>24.938461303710938</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="0">
+        <v>10</v>
+      </c>
+      <c r="G16" s="13">
+        <v>11</v>
+      </c>
+      <c r="H16" s="13">
+        <v>26.72307777404785</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="0">
+        <v>2</v>
+      </c>
+      <c r="G17" s="13">
+        <v>12</v>
+      </c>
+      <c r="H17" s="13">
+        <v>24.815383911132812</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="0">
+        <v>5</v>
+      </c>
+      <c r="G18" s="13">
+        <v>13</v>
+      </c>
+      <c r="H18" s="13">
+        <v>24.69230842590332</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="G19" s="13">
+        <v>14</v>
+      </c>
+      <c r="H19" s="13">
+        <v>28.72307777404785</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="G20" s="13">
+        <v>15</v>
+      </c>
+      <c r="H20" s="13">
+        <v>26.938461303710938</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="G21" s="13">
+        <v>16</v>
+      </c>
+      <c r="H21" s="13">
+        <v>28.72307777404785</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="G22" s="13">
+        <v>17</v>
+      </c>
+      <c r="H22" s="13">
+        <v>28.169231414794922</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="G23" s="13">
+        <v>18</v>
+      </c>
+      <c r="H23" s="13">
+        <v>25.5230770111084</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="G24" s="13">
+        <v>19</v>
+      </c>
+      <c r="H24" s="13">
+        <v>27.707693099975586</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="G25" s="13">
+        <v>20</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="G26" s="13">
+        <v>21</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="G27" s="13">
+        <v>22</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="G28" s="13">
+        <v>23</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="G29" s="13">
+        <v>24</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="G30" s="13">
+        <v>25</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="G31" s="13">
+        <v>26</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="G32" s="13">
+        <v>27</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="G33" s="13">
+        <v>28</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="G34" s="13">
+        <v>29</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="G35" s="13">
+        <v>30</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="G36" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" s="14">
+        <v>28.72307777404785</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="G37" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" s="14">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="G38" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38" s="14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="G39" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" s="14">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="G40" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells>
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName=""/>
+  <dimension ref="B5:H40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="9.4" customWidth="1"/>
+    <col min="7" max="7" width="20.3" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5">
+      <c r="B5" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="G5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="0">
+        <v>20</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13">
+        <v>12.770833015441895</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="0">
+        <v>30</v>
+      </c>
+      <c r="G7" s="13">
+        <v>2</v>
+      </c>
+      <c r="H7" s="13">
+        <v>18.33333396911621</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="0">
+        <v>100</v>
+      </c>
+      <c r="G8" s="13">
+        <v>3</v>
+      </c>
+      <c r="H8" s="13">
+        <v>21.73958396911621</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="0">
+        <v>5</v>
+      </c>
+      <c r="G9" s="13">
+        <v>4</v>
+      </c>
+      <c r="H9" s="13">
+        <v>21.625</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="0">
+        <v>6</v>
+      </c>
+      <c r="G10" s="13">
+        <v>5</v>
+      </c>
+      <c r="H10" s="13">
+        <v>20.58333396911621</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="0">
+        <v>12</v>
+      </c>
+      <c r="G11" s="13">
+        <v>6</v>
+      </c>
+      <c r="H11" s="13">
+        <v>22.66666603088379</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="0">
+        <v>21</v>
+      </c>
+      <c r="G12" s="13">
+        <v>7</v>
+      </c>
+      <c r="H12" s="13">
+        <v>22.36458396911621</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="0">
+        <v>50</v>
+      </c>
+      <c r="G13" s="13">
+        <v>8</v>
+      </c>
+      <c r="H13" s="13">
+        <v>23.92708396911621</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="0">
+        <v>25</v>
+      </c>
+      <c r="G14" s="13">
+        <v>9</v>
+      </c>
+      <c r="H14" s="13">
+        <v>26.53125</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="0">
+        <v>10</v>
+      </c>
+      <c r="G15" s="13">
+        <v>10</v>
+      </c>
+      <c r="H15" s="13">
+        <v>26.96875</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="0">
+        <v>10</v>
+      </c>
+      <c r="G16" s="13">
+        <v>11</v>
+      </c>
+      <c r="H16" s="13">
+        <v>27.92708396911621</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="0">
+        <v>2</v>
+      </c>
+      <c r="G17" s="13">
+        <v>12</v>
+      </c>
+      <c r="H17" s="13">
+        <v>33.35416793823242</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="0">
+        <v>5</v>
+      </c>
+      <c r="G18" s="13">
+        <v>13</v>
+      </c>
+      <c r="H18" s="13">
+        <v>29.13541603088379</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="G19" s="13">
+        <v>14</v>
+      </c>
+      <c r="H19" s="13">
+        <v>25.27083396911621</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="G20" s="13">
+        <v>15</v>
+      </c>
+      <c r="H20" s="13">
+        <v>26.01041603088379</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="G21" s="13">
+        <v>16</v>
+      </c>
+      <c r="H21" s="13">
+        <v>25.92708396911621</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="G22" s="13">
+        <v>17</v>
+      </c>
+      <c r="H22" s="13">
+        <v>29.27083396911621</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="G23" s="13">
+        <v>18</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="G24" s="13">
+        <v>19</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="G25" s="13">
+        <v>20</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="G26" s="13">
+        <v>21</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="G27" s="13">
+        <v>22</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="G28" s="13">
+        <v>23</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="G29" s="13">
+        <v>24</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="G30" s="13">
+        <v>25</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="G31" s="13">
+        <v>26</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="G32" s="13">
+        <v>27</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="G33" s="13">
+        <v>28</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="G34" s="13">
+        <v>29</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="G35" s="13">
+        <v>30</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="G36" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" s="14">
+        <v>33.35416793823242</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="G37" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" s="14">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="G38" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38" s="14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="G39" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" s="14">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="G40" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells>
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName=""/>
+  <dimension ref="B5:H40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="9.4" customWidth="1"/>
+    <col min="7" max="7" width="20.3" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5">
+      <c r="B5" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="G5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="0">
+        <v>20</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13">
+        <v>12.475409507751465</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="0">
+        <v>30</v>
+      </c>
+      <c r="G7" s="13">
+        <v>2</v>
+      </c>
+      <c r="H7" s="13">
+        <v>13.278688430786133</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="0">
+        <v>100</v>
+      </c>
+      <c r="G8" s="13">
+        <v>3</v>
+      </c>
+      <c r="H8" s="13">
+        <v>18.47541046142578</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="0">
+        <v>5</v>
+      </c>
+      <c r="G9" s="13">
+        <v>4</v>
+      </c>
+      <c r="H9" s="13">
+        <v>18.704917907714844</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="0">
+        <v>6</v>
+      </c>
+      <c r="G10" s="13">
+        <v>5</v>
+      </c>
+      <c r="H10" s="13">
+        <v>17.52458953857422</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="0">
+        <v>12</v>
+      </c>
+      <c r="G11" s="13">
+        <v>6</v>
+      </c>
+      <c r="H11" s="13">
+        <v>17.098360061645508</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="0">
+        <v>30</v>
+      </c>
+      <c r="G12" s="13">
+        <v>7</v>
+      </c>
+      <c r="H12" s="13">
+        <v>17.704917907714844</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="0">
+        <v>13</v>
+      </c>
+      <c r="G13" s="13">
+        <v>8</v>
+      </c>
+      <c r="H13" s="13">
+        <v>20.327869415283203</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="0">
+        <v>18</v>
+      </c>
+      <c r="G14" s="13">
+        <v>9</v>
+      </c>
+      <c r="H14" s="13">
+        <v>18.295082092285156</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="0">
+        <v>10</v>
+      </c>
+      <c r="G15" s="13">
+        <v>10</v>
+      </c>
+      <c r="H15" s="13">
+        <v>19.344263076782227</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="0">
+        <v>10</v>
+      </c>
+      <c r="G16" s="13">
+        <v>11</v>
+      </c>
+      <c r="H16" s="13">
+        <v>19.42622947692871</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="0">
+        <v>2</v>
+      </c>
+      <c r="G17" s="13">
+        <v>12</v>
+      </c>
+      <c r="H17" s="13">
+        <v>15.983606338500977</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="0">
+        <v>5</v>
+      </c>
+      <c r="G18" s="13">
+        <v>13</v>
+      </c>
+      <c r="H18" s="13">
+        <v>19.26229476928711</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="G19" s="13">
+        <v>14</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="G20" s="13">
+        <v>15</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="G21" s="13">
+        <v>16</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="G22" s="13">
+        <v>17</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="G23" s="13">
+        <v>18</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="G24" s="13">
+        <v>19</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="G25" s="13">
+        <v>20</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="G26" s="13">
+        <v>21</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="G27" s="13">
+        <v>22</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="G28" s="13">
+        <v>23</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="G29" s="13">
+        <v>24</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="G30" s="13">
+        <v>25</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="G31" s="13">
+        <v>26</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="G32" s="13">
+        <v>27</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="G33" s="13">
+        <v>28</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="G34" s="13">
+        <v>29</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="G35" s="13">
+        <v>30</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="G36" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" s="14">
+        <v>20.327869415283203</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="G37" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" s="14">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="G38" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38" s="14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="G39" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" s="14">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="G40" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells>
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName=""/>
+  <dimension ref="B5:N40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="9.4" customWidth="1"/>
+    <col min="7" max="7" width="20.3" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
+    <col min="11" max="11" width="21" customWidth="1"/>
+    <col min="12" max="12" width="21" customWidth="1"/>
+    <col min="13" max="13" width="21" customWidth="1"/>
+    <col min="14" max="14" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5">
+      <c r="B5" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="G5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="0">
+        <v>20</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13">
+        <v>13.666666984558105</v>
+      </c>
+      <c r="I6" s="13">
+        <v>13.666666984558105</v>
+      </c>
+      <c r="J6" s="13">
+        <v>13.666666984558105</v>
+      </c>
+      <c r="K6" s="13">
+        <v>13.666666984558105</v>
+      </c>
+      <c r="L6" s="13">
+        <v>13.666666984558105</v>
+      </c>
+      <c r="M6" s="13">
+        <v>13.666666984558105</v>
+      </c>
+      <c r="N6" s="13">
+        <v>13.666666984558105</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="0">
+        <v>30</v>
+      </c>
+      <c r="G7" s="13">
+        <v>2</v>
+      </c>
+      <c r="H7" s="13">
+        <v>14.666666984558105</v>
+      </c>
+      <c r="I7" s="13">
+        <v>14.666666984558105</v>
+      </c>
+      <c r="J7" s="13">
+        <v>14.666666984558105</v>
+      </c>
+      <c r="K7" s="13">
+        <v>14.666666984558105</v>
+      </c>
+      <c r="L7" s="13">
+        <v>14.666666984558105</v>
+      </c>
+      <c r="M7" s="13">
+        <v>14.666666984558105</v>
+      </c>
+      <c r="N7" s="13">
+        <v>14.666666984558105</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="0">
+        <v>100</v>
+      </c>
+      <c r="G8" s="13">
+        <v>3</v>
+      </c>
+      <c r="H8" s="13">
+        <v>17.33333396911621</v>
+      </c>
+      <c r="I8" s="13">
+        <v>17.33333396911621</v>
+      </c>
+      <c r="J8" s="13">
+        <v>17.33333396911621</v>
+      </c>
+      <c r="K8" s="13">
+        <v>17.33333396911621</v>
+      </c>
+      <c r="L8" s="13">
+        <v>17.33333396911621</v>
+      </c>
+      <c r="M8" s="13">
+        <v>17.33333396911621</v>
+      </c>
+      <c r="N8" s="13">
+        <v>17.33333396911621</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="0">
+        <v>5</v>
+      </c>
+      <c r="G9" s="13">
+        <v>4</v>
+      </c>
+      <c r="H9" s="13">
+        <v>18</v>
+      </c>
+      <c r="I9" s="13">
+        <v>18</v>
+      </c>
+      <c r="J9" s="13">
+        <v>18</v>
+      </c>
+      <c r="K9" s="13">
+        <v>18</v>
+      </c>
+      <c r="L9" s="13">
+        <v>18</v>
+      </c>
+      <c r="M9" s="13">
+        <v>18</v>
+      </c>
+      <c r="N9" s="13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="0">
+        <v>6</v>
+      </c>
+      <c r="G10" s="13">
+        <v>5</v>
+      </c>
+      <c r="H10" s="13">
+        <v>19</v>
+      </c>
+      <c r="I10" s="13">
+        <v>19</v>
+      </c>
+      <c r="J10" s="13">
+        <v>19</v>
+      </c>
+      <c r="K10" s="13">
+        <v>19</v>
+      </c>
+      <c r="L10" s="13">
+        <v>19</v>
+      </c>
+      <c r="M10" s="13">
+        <v>19</v>
+      </c>
+      <c r="N10" s="13">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="0">
+        <v>12</v>
+      </c>
+      <c r="G11" s="13">
+        <v>6</v>
+      </c>
+      <c r="H11" s="13">
+        <v>20.33333396911621</v>
+      </c>
+      <c r="I11" s="13">
+        <v>20.33333396911621</v>
+      </c>
+      <c r="J11" s="13">
+        <v>20.33333396911621</v>
+      </c>
+      <c r="K11" s="13">
+        <v>20.33333396911621</v>
+      </c>
+      <c r="L11" s="13">
+        <v>20.33333396911621</v>
+      </c>
+      <c r="M11" s="13">
+        <v>20.33333396911621</v>
+      </c>
+      <c r="N11" s="13">
+        <v>20.33333396911621</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="0">
+        <v>1</v>
+      </c>
+      <c r="G12" s="13">
+        <v>7</v>
+      </c>
+      <c r="H12" s="13">
+        <v>21</v>
+      </c>
+      <c r="I12" s="13">
+        <v>21</v>
+      </c>
+      <c r="J12" s="13">
+        <v>21</v>
+      </c>
+      <c r="K12" s="13">
+        <v>21</v>
+      </c>
+      <c r="L12" s="13">
+        <v>21</v>
+      </c>
+      <c r="M12" s="13">
+        <v>21</v>
+      </c>
+      <c r="N12" s="13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="0">
+        <v>1</v>
+      </c>
+      <c r="G13" s="13">
+        <v>8</v>
+      </c>
+      <c r="H13" s="13">
+        <v>21.66666603088379</v>
+      </c>
+      <c r="I13" s="13">
+        <v>21.66666603088379</v>
+      </c>
+      <c r="J13" s="13">
+        <v>21.66666603088379</v>
+      </c>
+      <c r="K13" s="13">
+        <v>21.66666603088379</v>
+      </c>
+      <c r="L13" s="13">
+        <v>21.66666603088379</v>
+      </c>
+      <c r="M13" s="13">
+        <v>21.66666603088379</v>
+      </c>
+      <c r="N13" s="13">
+        <v>21.66666603088379</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="0">
+        <v>1</v>
+      </c>
+      <c r="G14" s="13">
+        <v>9</v>
+      </c>
+      <c r="H14" s="13">
+        <v>25</v>
+      </c>
+      <c r="I14" s="13">
+        <v>25</v>
+      </c>
+      <c r="J14" s="13">
+        <v>25</v>
+      </c>
+      <c r="K14" s="13">
+        <v>25</v>
+      </c>
+      <c r="L14" s="13">
+        <v>25</v>
+      </c>
+      <c r="M14" s="13">
+        <v>25</v>
+      </c>
+      <c r="N14" s="13">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="0">
+        <v>10</v>
+      </c>
+      <c r="G15" s="13">
+        <v>10</v>
+      </c>
+      <c r="H15" s="13">
+        <v>21.66666603088379</v>
+      </c>
+      <c r="I15" s="13">
+        <v>21.66666603088379</v>
+      </c>
+      <c r="J15" s="13">
+        <v>21.66666603088379</v>
+      </c>
+      <c r="K15" s="13">
+        <v>21.66666603088379</v>
+      </c>
+      <c r="L15" s="13">
+        <v>21.66666603088379</v>
+      </c>
+      <c r="M15" s="13">
+        <v>21.66666603088379</v>
+      </c>
+      <c r="N15" s="13">
+        <v>21.66666603088379</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="0">
+        <v>10</v>
+      </c>
+      <c r="G16" s="13">
+        <v>11</v>
+      </c>
+      <c r="H16" s="13">
+        <v>23</v>
+      </c>
+      <c r="I16" s="13">
+        <v>23</v>
+      </c>
+      <c r="J16" s="13">
+        <v>23</v>
+      </c>
+      <c r="K16" s="13">
+        <v>23</v>
+      </c>
+      <c r="L16" s="13">
+        <v>23</v>
+      </c>
+      <c r="M16" s="13">
+        <v>23</v>
+      </c>
+      <c r="N16" s="13">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="0">
+        <v>2</v>
+      </c>
+      <c r="G17" s="13">
+        <v>12</v>
+      </c>
+      <c r="H17" s="13">
+        <v>22</v>
+      </c>
+      <c r="I17" s="13">
+        <v>22</v>
+      </c>
+      <c r="J17" s="13">
+        <v>22</v>
+      </c>
+      <c r="K17" s="13">
+        <v>22</v>
+      </c>
+      <c r="L17" s="13">
+        <v>22</v>
+      </c>
+      <c r="M17" s="13">
+        <v>22</v>
+      </c>
+      <c r="N17" s="13">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="0">
+        <v>5</v>
+      </c>
+      <c r="G18" s="13">
+        <v>13</v>
+      </c>
+      <c r="H18" s="13">
+        <v>23</v>
+      </c>
+      <c r="I18" s="13">
+        <v>23</v>
+      </c>
+      <c r="J18" s="13">
+        <v>23</v>
+      </c>
+      <c r="K18" s="13">
+        <v>23</v>
+      </c>
+      <c r="L18" s="13">
+        <v>23</v>
+      </c>
+      <c r="M18" s="13">
+        <v>23</v>
+      </c>
+      <c r="N18" s="13">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="G19" s="13">
+        <v>14</v>
+      </c>
+      <c r="H19" s="13">
+        <v>24.66666603088379</v>
+      </c>
+      <c r="I19" s="13">
+        <v>24.66666603088379</v>
+      </c>
+      <c r="J19" s="13">
+        <v>24.66666603088379</v>
+      </c>
+      <c r="K19" s="13">
+        <v>24.66666603088379</v>
+      </c>
+      <c r="L19" s="13">
+        <v>24.66666603088379</v>
+      </c>
+      <c r="M19" s="13">
+        <v>24.66666603088379</v>
+      </c>
+      <c r="N19" s="13">
+        <v>24.66666603088379</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="G20" s="13">
+        <v>15</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M20" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="N20" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="G21" s="13">
+        <v>16</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M21" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="N21" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="G22" s="13">
+        <v>17</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="N22" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="G23" s="13">
+        <v>18</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L23" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M23" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="N23" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="G24" s="13">
+        <v>19</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L24" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M24" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="N24" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="G25" s="13">
+        <v>20</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K25" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M25" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="N25" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="G26" s="13">
+        <v>21</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M26" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="N26" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="G27" s="13">
+        <v>22</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J27" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K27" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L27" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M27" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="N27" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="G28" s="13">
+        <v>23</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J28" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K28" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L28" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M28" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="N28" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="G29" s="13">
+        <v>24</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J29" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K29" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L29" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M29" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="N29" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="G30" s="13">
+        <v>25</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="N30" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="G31" s="13">
+        <v>26</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J31" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K31" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L31" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M31" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="N31" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="G32" s="13">
+        <v>27</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="N32" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="G33" s="13">
+        <v>28</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J33" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K33" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L33" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M33" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="N33" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="G34" s="13">
+        <v>29</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J34" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K34" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L34" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M34" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="N34" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="G35" s="13">
+        <v>30</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J35" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K35" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L35" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M35" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="N35" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="G36" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" s="14">
+        <v>25</v>
+      </c>
+      <c r="I36" s="14">
+        <v>25</v>
+      </c>
+      <c r="J36" s="14">
+        <v>25</v>
+      </c>
+      <c r="K36" s="14">
+        <v>25</v>
+      </c>
+      <c r="L36" s="14">
+        <v>25</v>
+      </c>
+      <c r="M36" s="14">
+        <v>25</v>
+      </c>
+      <c r="N36" s="14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="G37" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" s="14">
+        <v>24</v>
+      </c>
+      <c r="I37" s="14">
+        <v>24</v>
+      </c>
+      <c r="J37" s="14">
+        <v>24</v>
+      </c>
+      <c r="K37" s="14">
+        <v>24</v>
+      </c>
+      <c r="L37" s="14">
+        <v>24</v>
+      </c>
+      <c r="M37" s="14">
+        <v>24</v>
+      </c>
+      <c r="N37" s="14">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="G38" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38" s="14">
+        <v>11</v>
+      </c>
+      <c r="I38" s="14">
+        <v>11</v>
+      </c>
+      <c r="J38" s="14">
+        <v>11</v>
+      </c>
+      <c r="K38" s="14">
+        <v>11</v>
+      </c>
+      <c r="L38" s="14">
+        <v>11</v>
+      </c>
+      <c r="M38" s="14">
+        <v>11</v>
+      </c>
+      <c r="N38" s="14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="G39" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" s="14">
+        <v>40</v>
+      </c>
+      <c r="I39" s="14">
+        <v>40</v>
+      </c>
+      <c r="J39" s="14">
+        <v>40</v>
+      </c>
+      <c r="K39" s="14">
+        <v>40</v>
+      </c>
+      <c r="L39" s="14">
+        <v>40</v>
+      </c>
+      <c r="M39" s="14">
+        <v>40</v>
+      </c>
+      <c r="N39" s="14">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="G40" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I40" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="J40" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="K40" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="L40" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="M40" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="N40" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells>
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName=""/>
+  <dimension ref="B5:K40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="34" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="7" max="7" width="20.3" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
+    <col min="11" max="11" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5">
+      <c r="B5" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="G5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="19">
+        <v>20</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13">
+        <v>14.174603462219238</v>
+      </c>
+      <c r="I6" s="13">
+        <v>7.55555534362793</v>
+      </c>
+      <c r="J6" s="13">
+        <v>11.619047164916992</v>
+      </c>
+      <c r="K6" s="13">
+        <v>15.380952835083008</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="19">
+        <v>30</v>
+      </c>
+      <c r="G7" s="13">
+        <v>2</v>
+      </c>
+      <c r="H7" s="13">
+        <v>19.44444465637207</v>
+      </c>
+      <c r="I7" s="13">
+        <v>15.920635223388672</v>
+      </c>
+      <c r="J7" s="13">
+        <v>15.063491821289062</v>
+      </c>
+      <c r="K7" s="13">
+        <v>14.809523582458496</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="19">
+        <v>100</v>
+      </c>
+      <c r="G8" s="13">
+        <v>3</v>
+      </c>
+      <c r="H8" s="13">
+        <v>17.44444465637207</v>
+      </c>
+      <c r="I8" s="13">
+        <v>21.206348419189453</v>
+      </c>
+      <c r="J8" s="13">
+        <v>18.507936477661133</v>
+      </c>
+      <c r="K8" s="13">
+        <v>20.952381134033203</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="19">
+        <v>5</v>
+      </c>
+      <c r="G9" s="13">
+        <v>4</v>
+      </c>
+      <c r="H9" s="13">
+        <v>24.396825790405273</v>
+      </c>
+      <c r="I9" s="13">
+        <v>22.190475463867188</v>
+      </c>
+      <c r="J9" s="13">
+        <v>16.126983642578125</v>
+      </c>
+      <c r="K9" s="13">
+        <v>19.73015785217285</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="19">
+        <v>6</v>
+      </c>
+      <c r="G10" s="13">
+        <v>5</v>
+      </c>
+      <c r="H10" s="13">
+        <v>25.936508178710938</v>
+      </c>
+      <c r="I10" s="13">
+        <v>23.30158805847168</v>
+      </c>
+      <c r="J10" s="13">
+        <v>25.58730125427246</v>
+      </c>
+      <c r="K10" s="13">
+        <v>21.746030807495117</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="19">
+        <v>12</v>
+      </c>
+      <c r="G11" s="13">
+        <v>6</v>
+      </c>
+      <c r="H11" s="13">
+        <v>26.428571701049805</v>
+      </c>
+      <c r="I11" s="13">
+        <v>23.793651580810547</v>
+      </c>
+      <c r="J11" s="13">
+        <v>25.904762268066406</v>
+      </c>
+      <c r="K11" s="13">
+        <v>22.4761905670166</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="19">
+        <v>21</v>
+      </c>
+      <c r="G12" s="13">
+        <v>7</v>
+      </c>
+      <c r="H12" s="13">
+        <v>26.460317611694336</v>
+      </c>
+      <c r="I12" s="13">
+        <v>25.761905670166016</v>
+      </c>
+      <c r="J12" s="13">
+        <v>24.920635223388672</v>
+      </c>
+      <c r="K12" s="13">
+        <v>24.603174209594727</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="19">
+        <v>31</v>
+      </c>
+      <c r="G13" s="13">
+        <v>8</v>
+      </c>
+      <c r="H13" s="13">
+        <v>23.492063522338867</v>
+      </c>
+      <c r="I13" s="13">
+        <v>28.571428298950195</v>
+      </c>
+      <c r="J13" s="13">
+        <v>27.253969192504883</v>
+      </c>
+      <c r="K13" s="13">
+        <v>26.41269874572754</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="19">
+        <v>11</v>
+      </c>
+      <c r="G14" s="13">
+        <v>9</v>
+      </c>
+      <c r="H14" s="13">
+        <v>25.317461013793945</v>
+      </c>
+      <c r="I14" s="13">
+        <v>23.650793075561523</v>
+      </c>
+      <c r="J14" s="13">
+        <v>23.920635223388672</v>
+      </c>
+      <c r="K14" s="13">
+        <v>26.460317611694336</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="19">
+        <v>10</v>
+      </c>
+      <c r="G15" s="13">
+        <v>10</v>
+      </c>
+      <c r="H15" s="13">
+        <v>23.539682388305664</v>
+      </c>
+      <c r="I15" s="13">
+        <v>29.063491821289062</v>
+      </c>
+      <c r="J15" s="13">
+        <v>26.920635223388672</v>
+      </c>
+      <c r="K15" s="13">
+        <v>26.746030807495117</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="19">
+        <v>10</v>
+      </c>
+      <c r="G16" s="13">
+        <v>11</v>
+      </c>
+      <c r="H16" s="13">
+        <v>25.96825408935547</v>
+      </c>
+      <c r="I16" s="13">
+        <v>25.190475463867188</v>
+      </c>
+      <c r="J16" s="13">
+        <v>26.015872955322266</v>
+      </c>
+      <c r="K16" s="13">
+        <v>24.33333396911621</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="19">
+        <v>2</v>
+      </c>
+      <c r="G17" s="13">
+        <v>12</v>
+      </c>
+      <c r="H17" s="13">
+        <v>26.650793075561523</v>
+      </c>
+      <c r="I17" s="13">
+        <v>23.793651580810547</v>
+      </c>
+      <c r="J17" s="13">
+        <v>28.571428298950195</v>
+      </c>
+      <c r="K17" s="13">
+        <v>23.349206924438477</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="19">
+        <v>5</v>
+      </c>
+      <c r="G18" s="13">
+        <v>13</v>
+      </c>
+      <c r="H18" s="13">
+        <v>27.14285659790039</v>
+      </c>
+      <c r="I18" s="13">
+        <v>27.396825790405273</v>
+      </c>
+      <c r="J18" s="13">
+        <v>29.55555534362793</v>
+      </c>
+      <c r="K18" s="13">
+        <v>26.26984214782715</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="13">
+        <v>14</v>
+      </c>
+      <c r="H19" s="13">
+        <v>27.619047164916992</v>
+      </c>
+      <c r="I19" s="13">
+        <v>29.047618865966797</v>
+      </c>
+      <c r="J19" s="13">
+        <v>23.126983642578125</v>
+      </c>
+      <c r="K19" s="13">
+        <v>27.41269874572754</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="13">
+        <v>15</v>
+      </c>
+      <c r="H20" s="13">
+        <v>29.190475463867188</v>
+      </c>
+      <c r="I20" s="13">
+        <v>27.603174209594727</v>
+      </c>
+      <c r="J20" s="13">
+        <v>24.904762268066406</v>
+      </c>
+      <c r="K20" s="13">
+        <v>29.873016357421875</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" s="13">
+        <v>16</v>
+      </c>
+      <c r="H21" s="13">
+        <v>29.190475463867188</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" s="13">
+        <v>26.714284896850586</v>
+      </c>
+      <c r="K21" s="13">
+        <v>27.539682388305664</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="G22" s="13">
+        <v>17</v>
+      </c>
+      <c r="H22" s="13">
+        <v>29.063491821289062</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" s="13">
+        <v>26</v>
+      </c>
+      <c r="K22" s="13">
+        <v>27.88888931274414</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="G23" s="13">
+        <v>18</v>
+      </c>
+      <c r="H23" s="13">
+        <v>27.58730125427246</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" s="13">
+        <v>26.761905670166016</v>
+      </c>
+      <c r="K23" s="13">
+        <v>28.079364776611328</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="G24" s="13">
+        <v>19</v>
+      </c>
+      <c r="H24" s="13">
+        <v>31.5238094329834</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="13">
+        <v>26.88888931274414</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="G25" s="13">
+        <v>20</v>
+      </c>
+      <c r="H25" s="13">
+        <v>30.539682388305664</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K25" s="13">
+        <v>28.365079879760742</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="G26" s="13">
+        <v>21</v>
+      </c>
+      <c r="H26" s="13">
+        <v>31.5238094329834</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="G27" s="13">
+        <v>22</v>
+      </c>
+      <c r="H27" s="13">
+        <v>28.761905670166016</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J27" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K27" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="G28" s="13">
+        <v>23</v>
+      </c>
+      <c r="H28" s="13">
+        <v>30.30158805847168</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J28" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K28" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="G29" s="13">
+        <v>24</v>
+      </c>
+      <c r="H29" s="13">
+        <v>30.238094329833984</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J29" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K29" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="G30" s="13">
+        <v>25</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="G31" s="13">
+        <v>26</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J31" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K31" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="G32" s="13">
+        <v>27</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K32" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="G33" s="13">
+        <v>28</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J33" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K33" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="G34" s="13">
+        <v>29</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J34" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K34" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="G35" s="13">
+        <v>30</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J35" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K35" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="G36" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" s="14">
+        <v>31.5238094329834</v>
+      </c>
+      <c r="I36" s="14">
+        <v>29.063491821289062</v>
+      </c>
+      <c r="J36" s="14">
+        <v>29.55555534362793</v>
+      </c>
+      <c r="K36" s="14">
+        <v>29.873016357421875</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="G37" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" s="14">
+        <v>15</v>
+      </c>
+      <c r="I37" s="14">
+        <v>6</v>
+      </c>
+      <c r="J37" s="14">
+        <v>28</v>
+      </c>
+      <c r="K37" s="14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="G38" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38" s="14">
+        <v>7</v>
+      </c>
+      <c r="I38" s="14">
+        <v>3</v>
+      </c>
+      <c r="J38" s="14">
+        <v>12</v>
+      </c>
+      <c r="K38" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="G39" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" s="14">
+        <v>54</v>
+      </c>
+      <c r="I39" s="14">
+        <v>61</v>
+      </c>
+      <c r="J39" s="14">
+        <v>42</v>
+      </c>
+      <c r="K39" s="14">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="G40" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I40" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="J40" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K40" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells>
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Aggiunto il menù dei dati dell'algoritmo genetico e migliore telecamera
- Aggiunti i metodi per zoomare e muovere la telecamera di gioco
- Aggiunto il menù per visualizzare i dati di output dell'algoritmo genetico
- Aggiunto il metodo per controllare se l'algoritmo è in corso e quindi disabilitare il bottone di generazione di una nuova mappa
</commit_message>
<xml_diff>
--- a/Genetic Map Generation/Data/GAData.xlsx
+++ b/Genetic Map Generation/Data/GAData.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Configurazione Algoritmo Genetico</t>
   </si>
@@ -210,6 +210,15 @@
   </si>
   <si>
     <t>00:00:00:11612</t>
+  </si>
+  <si>
+    <t>00:00:00:14274</t>
+  </si>
+  <si>
+    <t>00:00:00:08134</t>
+  </si>
+  <si>
+    <t>00:00:00:16550</t>
   </si>
 </sst>
 </file>
@@ -3521,7 +3530,7 @@
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="B5:I40"/>
+  <dimension ref="B5:L40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3532,6 +3541,9 @@
     <col min="7" max="7" width="20.3" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
+    <col min="11" max="11" width="21" customWidth="1"/>
+    <col min="12" max="12" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5">
@@ -3548,6 +3560,15 @@
       <c r="I5" s="26" t="s">
         <v>2</v>
       </c>
+      <c r="J5" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="26" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="21" t="s">
@@ -3565,6 +3586,15 @@
       <c r="I6" s="25">
         <v>16.66666603088379</v>
       </c>
+      <c r="J6" s="25">
+        <v>15</v>
+      </c>
+      <c r="K6" s="25">
+        <v>5.666666507720947</v>
+      </c>
+      <c r="L6" s="25">
+        <v>14.333333015441895</v>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="21" t="s">
@@ -3582,6 +3612,15 @@
       <c r="I7" s="25">
         <v>18.33333396911621</v>
       </c>
+      <c r="J7" s="25">
+        <v>17.66666603088379</v>
+      </c>
+      <c r="K7" s="25">
+        <v>11.333333015441895</v>
+      </c>
+      <c r="L7" s="25">
+        <v>14.666666984558105</v>
+      </c>
     </row>
     <row r="8">
       <c r="B8" s="21" t="s">
@@ -3599,6 +3638,15 @@
       <c r="I8" s="25">
         <v>20.66666603088379</v>
       </c>
+      <c r="J8" s="25">
+        <v>19.33333396911621</v>
+      </c>
+      <c r="K8" s="25">
+        <v>13.333333015441895</v>
+      </c>
+      <c r="L8" s="25">
+        <v>16.66666603088379</v>
+      </c>
     </row>
     <row r="9">
       <c r="B9" s="21" t="s">
@@ -3616,6 +3664,15 @@
       <c r="I9" s="25">
         <v>20</v>
       </c>
+      <c r="J9" s="25">
+        <v>20.33333396911621</v>
+      </c>
+      <c r="K9" s="25">
+        <v>20.66666603088379</v>
+      </c>
+      <c r="L9" s="25">
+        <v>18</v>
+      </c>
     </row>
     <row r="10">
       <c r="B10" s="21" t="s">
@@ -3633,6 +3690,15 @@
       <c r="I10" s="25">
         <v>21.66666603088379</v>
       </c>
+      <c r="J10" s="25">
+        <v>23</v>
+      </c>
+      <c r="K10" s="25">
+        <v>24.66666603088379</v>
+      </c>
+      <c r="L10" s="25">
+        <v>20</v>
+      </c>
     </row>
     <row r="11">
       <c r="B11" s="21" t="s">
@@ -3650,6 +3716,15 @@
       <c r="I11" s="25">
         <v>23.66666603088379</v>
       </c>
+      <c r="J11" s="25">
+        <v>22.33333396911621</v>
+      </c>
+      <c r="K11" s="25">
+        <v>25.66666603088379</v>
+      </c>
+      <c r="L11" s="25">
+        <v>22.33333396911621</v>
+      </c>
     </row>
     <row r="12">
       <c r="B12" s="21" t="s">
@@ -3667,6 +3742,15 @@
       <c r="I12" s="25">
         <v>24.33333396911621</v>
       </c>
+      <c r="J12" s="25">
+        <v>22.66666603088379</v>
+      </c>
+      <c r="K12" s="25">
+        <v>21</v>
+      </c>
+      <c r="L12" s="25">
+        <v>21.33333396911621</v>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="21" t="s">
@@ -3684,6 +3768,15 @@
       <c r="I13" s="25">
         <v>24.66666603088379</v>
       </c>
+      <c r="J13" s="25">
+        <v>23.33333396911621</v>
+      </c>
+      <c r="K13" s="25">
+        <v>21.66666603088379</v>
+      </c>
+      <c r="L13" s="25">
+        <v>23.33333396911621</v>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="21" t="s">
@@ -3701,6 +3794,15 @@
       <c r="I14" s="25">
         <v>24.33333396911621</v>
       </c>
+      <c r="J14" s="25">
+        <v>19.66666603088379</v>
+      </c>
+      <c r="K14" s="25">
+        <v>22.33333396911621</v>
+      </c>
+      <c r="L14" s="25">
+        <v>23</v>
+      </c>
     </row>
     <row r="15">
       <c r="B15" s="21" t="s">
@@ -3718,6 +3820,15 @@
       <c r="I15" s="25">
         <v>24.66666603088379</v>
       </c>
+      <c r="J15" s="25">
+        <v>24.66666603088379</v>
+      </c>
+      <c r="K15" s="25">
+        <v>22.66666603088379</v>
+      </c>
+      <c r="L15" s="25">
+        <v>23.33333396911621</v>
+      </c>
     </row>
     <row r="16">
       <c r="B16" s="21" t="s">
@@ -3735,6 +3846,15 @@
       <c r="I16" s="25">
         <v>22</v>
       </c>
+      <c r="J16" s="25">
+        <v>23.66666603088379</v>
+      </c>
+      <c r="K16" s="25">
+        <v>25.33333396911621</v>
+      </c>
+      <c r="L16" s="25">
+        <v>24.33333396911621</v>
+      </c>
     </row>
     <row r="17">
       <c r="B17" s="21" t="s">
@@ -3752,6 +3872,15 @@
       <c r="I17" s="25">
         <v>23</v>
       </c>
+      <c r="J17" s="25">
+        <v>24.33333396911621</v>
+      </c>
+      <c r="K17" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" s="25">
+        <v>23.66666603088379</v>
+      </c>
     </row>
     <row r="18">
       <c r="B18" s="21" t="s">
@@ -3769,6 +3898,15 @@
       <c r="I18" s="25">
         <v>23.33333396911621</v>
       </c>
+      <c r="J18" s="25">
+        <v>24.66666603088379</v>
+      </c>
+      <c r="K18" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L18" s="25">
+        <v>22.66666603088379</v>
+      </c>
     </row>
     <row r="19">
       <c r="B19" s="21" t="s">
@@ -3786,6 +3924,15 @@
       <c r="I19" s="25" t="s">
         <v>16</v>
       </c>
+      <c r="J19" s="25">
+        <v>24.66666603088379</v>
+      </c>
+      <c r="K19" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L19" s="25">
+        <v>23.33333396911621</v>
+      </c>
     </row>
     <row r="20">
       <c r="B20" s="21" t="s">
@@ -3803,6 +3950,15 @@
       <c r="I20" s="25" t="s">
         <v>16</v>
       </c>
+      <c r="J20" s="25">
+        <v>25</v>
+      </c>
+      <c r="K20" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L20" s="25">
+        <v>25</v>
+      </c>
     </row>
     <row r="21">
       <c r="B21" s="22" t="s">
@@ -3820,6 +3976,15 @@
       <c r="I21" s="25" t="s">
         <v>16</v>
       </c>
+      <c r="J21" s="25">
+        <v>24.66666603088379</v>
+      </c>
+      <c r="K21" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L21" s="25">
+        <v>25</v>
+      </c>
     </row>
     <row r="22">
       <c r="G22" s="25">
@@ -3831,6 +3996,15 @@
       <c r="I22" s="25" t="s">
         <v>16</v>
       </c>
+      <c r="J22" s="25">
+        <v>24.33333396911621</v>
+      </c>
+      <c r="K22" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L22" s="25">
+        <v>23.66666603088379</v>
+      </c>
     </row>
     <row r="23">
       <c r="G23" s="25">
@@ -3842,6 +4016,15 @@
       <c r="I23" s="25" t="s">
         <v>16</v>
       </c>
+      <c r="J23" s="25">
+        <v>25</v>
+      </c>
+      <c r="K23" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L23" s="25">
+        <v>23.33333396911621</v>
+      </c>
     </row>
     <row r="24">
       <c r="G24" s="25">
@@ -3853,6 +4036,15 @@
       <c r="I24" s="25" t="s">
         <v>16</v>
       </c>
+      <c r="J24" s="25">
+        <v>23.66666603088379</v>
+      </c>
+      <c r="K24" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L24" s="25">
+        <v>23</v>
+      </c>
     </row>
     <row r="25">
       <c r="G25" s="25">
@@ -3864,6 +4056,15 @@
       <c r="I25" s="25" t="s">
         <v>16</v>
       </c>
+      <c r="J25" s="25">
+        <v>23.33333396911621</v>
+      </c>
+      <c r="K25" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L25" s="25">
+        <v>24.66666603088379</v>
+      </c>
     </row>
     <row r="26">
       <c r="G26" s="25">
@@ -3875,6 +4076,15 @@
       <c r="I26" s="25" t="s">
         <v>16</v>
       </c>
+      <c r="J26" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L26" s="25" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="27">
       <c r="G27" s="25">
@@ -3886,6 +4096,15 @@
       <c r="I27" s="25" t="s">
         <v>16</v>
       </c>
+      <c r="J27" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="K27" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L27" s="25" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="28">
       <c r="G28" s="25">
@@ -3897,6 +4116,15 @@
       <c r="I28" s="25" t="s">
         <v>16</v>
       </c>
+      <c r="J28" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="K28" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L28" s="25" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="29">
       <c r="G29" s="25">
@@ -3908,6 +4136,15 @@
       <c r="I29" s="25" t="s">
         <v>16</v>
       </c>
+      <c r="J29" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="K29" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L29" s="25" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="30">
       <c r="G30" s="25">
@@ -3919,6 +4156,15 @@
       <c r="I30" s="25" t="s">
         <v>16</v>
       </c>
+      <c r="J30" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L30" s="25" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="31">
       <c r="G31" s="25">
@@ -3930,6 +4176,15 @@
       <c r="I31" s="25" t="s">
         <v>16</v>
       </c>
+      <c r="J31" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="K31" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L31" s="25" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="32">
       <c r="G32" s="25">
@@ -3941,6 +4196,15 @@
       <c r="I32" s="25" t="s">
         <v>16</v>
       </c>
+      <c r="J32" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="K32" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L32" s="25" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="33">
       <c r="G33" s="25">
@@ -3952,6 +4216,15 @@
       <c r="I33" s="25" t="s">
         <v>16</v>
       </c>
+      <c r="J33" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="K33" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L33" s="25" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="34">
       <c r="G34" s="25">
@@ -3963,6 +4236,15 @@
       <c r="I34" s="25" t="s">
         <v>16</v>
       </c>
+      <c r="J34" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="K34" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L34" s="25" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="35">
       <c r="G35" s="25">
@@ -3974,6 +4256,15 @@
       <c r="I35" s="25" t="s">
         <v>16</v>
       </c>
+      <c r="J35" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="K35" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L35" s="25" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="36">
       <c r="G36" s="27" t="s">
@@ -3985,6 +4276,15 @@
       <c r="I36" s="27">
         <v>24.66666603088379</v>
       </c>
+      <c r="J36" s="27">
+        <v>25</v>
+      </c>
+      <c r="K36" s="27">
+        <v>25.66666603088379</v>
+      </c>
+      <c r="L36" s="27">
+        <v>25</v>
+      </c>
     </row>
     <row r="37">
       <c r="G37" s="27" t="s">
@@ -3996,6 +4296,15 @@
       <c r="I37" s="27">
         <v>20</v>
       </c>
+      <c r="J37" s="27">
+        <v>20</v>
+      </c>
+      <c r="K37" s="27">
+        <v>31</v>
+      </c>
+      <c r="L37" s="27">
+        <v>24</v>
+      </c>
     </row>
     <row r="38">
       <c r="G38" s="27" t="s">
@@ -4007,6 +4316,15 @@
       <c r="I38" s="27">
         <v>12</v>
       </c>
+      <c r="J38" s="27">
+        <v>12</v>
+      </c>
+      <c r="K38" s="27">
+        <v>12</v>
+      </c>
+      <c r="L38" s="27">
+        <v>12</v>
+      </c>
     </row>
     <row r="39">
       <c r="G39" s="27" t="s">
@@ -4018,6 +4336,15 @@
       <c r="I39" s="27">
         <v>42</v>
       </c>
+      <c r="J39" s="27">
+        <v>43</v>
+      </c>
+      <c r="K39" s="27">
+        <v>34</v>
+      </c>
+      <c r="L39" s="27">
+        <v>39</v>
+      </c>
     </row>
     <row r="40">
       <c r="G40" s="27" t="s">
@@ -4028,6 +4355,15 @@
       </c>
       <c r="I40" s="27" t="s">
         <v>53</v>
+      </c>
+      <c r="J40" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="K40" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="L40" s="27" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>